<commit_message>
Updates to documentation files ahead of rename/merge day
</commit_message>
<xml_diff>
--- a/documentation_files/documentation_tables.xlsx
+++ b/documentation_files/documentation_tables.xlsx
@@ -5,22 +5,29 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stateofwa-my.sharepoint.com/personal/evan_booher_dfw_wa_gov/Documents/code/CreelPointEstimate/docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stateofwa-my.sharepoint.com/personal/evan_booher_dfw_wa_gov/Documents/code/CreelPointEstimate/documentation_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="106" documentId="13_ncr:1_{06BDCB52-A10A-4652-9501-BAA58E581D65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A0398F24-454D-43F9-98DD-7ECDBFDE1231}"/>
+  <xr:revisionPtr revIDLastSave="501" documentId="13_ncr:1_{06BDCB52-A10A-4652-9501-BAA58E581D65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{148507F9-1DE4-47B8-B230-7B33B1931884}"/>
   <bookViews>
-    <workbookView xWindow="3825" yWindow="1065" windowWidth="22260" windowHeight="11910" firstSheet="3" activeTab="7" xr2:uid="{D87A213F-20EA-453F-96F1-E2F9D588DE08}"/>
+    <workbookView xWindow="2025" yWindow="1365" windowWidth="25875" windowHeight="13545" xr2:uid="{D87A213F-20EA-453F-96F1-E2F9D588DE08}"/>
   </bookViews>
   <sheets>
     <sheet name="design_stratification" sheetId="7" r:id="rId1"/>
     <sheet name="pre_analysis_checklist" sheetId="1" r:id="rId2"/>
     <sheet name="YAML_parameters" sheetId="2" r:id="rId3"/>
-    <sheet name="dwg_summ_interview" sheetId="4" r:id="rId4"/>
-    <sheet name="dwg_summ_effort_index" sheetId="6" r:id="rId5"/>
-    <sheet name="dwg_summ_effort_census" sheetId="5" r:id="rId6"/>
-    <sheet name="PE_effort" sheetId="3" r:id="rId7"/>
-    <sheet name="PE_catch" sheetId="8" r:id="rId8"/>
+    <sheet name="YAML_param_options" sheetId="9" r:id="rId4"/>
+    <sheet name="dwg_summ_interview" sheetId="4" r:id="rId5"/>
+    <sheet name="fetch_days_output" sheetId="10" r:id="rId6"/>
+    <sheet name="dwg_summ_effort_index" sheetId="6" r:id="rId7"/>
+    <sheet name="dwg_summ_effort_census" sheetId="5" r:id="rId8"/>
+    <sheet name="inputs_pe_ang_hours_daily_mean" sheetId="11" r:id="rId9"/>
+    <sheet name="inputs_pe$angler_per_vehicle_tr" sheetId="12" r:id="rId10"/>
+    <sheet name="inputs_pe$census" sheetId="13" r:id="rId11"/>
+    <sheet name="inputs_pe$days_total" sheetId="14" r:id="rId12"/>
+    <sheet name="inputs_pe$df" sheetId="15" r:id="rId13"/>
+    <sheet name="PE_effort" sheetId="3" r:id="rId14"/>
+    <sheet name="PE_catch" sheetId="8" r:id="rId15"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="194">
   <si>
     <t>Data is stored in the creel database and accessible from data.wa.gov</t>
   </si>
@@ -109,42 +116,6 @@
     <t>dir_output</t>
   </si>
   <si>
-    <t>character string with waterbody area, focal species, year / year-group to describe distinct creel project</t>
-  </si>
-  <si>
-    <t>minimum date of observations fetched from data.wa.gov</t>
-  </si>
-  <si>
-    <t>maximum date of observaitons fetched from data.wa.gov</t>
-  </si>
-  <si>
-    <t>specification of one or more groups of focal species, life stage, mark status, and encounter types of interest</t>
-  </si>
-  <si>
-    <t>specification designating method used to count anglers during census surveys, either counting the total number of people in angler groups ("group") or counting only people observed actively fishing ("angler")</t>
-  </si>
-  <si>
-    <t>time period for aggregation of observations; for period_pe options are: "week", "month", and "duration"</t>
-  </si>
-  <si>
-    <t>time period for aggregation of observations; for period_bss options are: "day" and "week"</t>
-  </si>
-  <si>
-    <t>Days assigned to "weekend" day type group (weekend or weekday)</t>
-  </si>
-  <si>
-    <t>specification for objects that are counted during index effort counts, either "Vehicle/Trailers Only" or "Bank Angler / Boat Angler"</t>
-  </si>
-  <si>
-    <t>Option to use either observed census data ("Direct") or assumed values ("Indirect") to calculate the effort bias term ratio</t>
-  </si>
-  <si>
-    <t>The minimum fishing time per angler group interview that is retained to calculate catch rates</t>
-  </si>
-  <si>
-    <t>directory name in file path where output from script is saved</t>
-  </si>
-  <si>
     <t>field</t>
   </si>
   <si>
@@ -232,12 +203,6 @@
     <t>Categorical value to assess the status of trip, either "complete" or "incomplete"</t>
   </si>
   <si>
-    <t>boolean value determining if the angler group was interviewed by a WDFW creel sampler earlier in the day</t>
-  </si>
-  <si>
-    <t>character string representing catch group of interest specified in the YAML metadata of the script</t>
-  </si>
-  <si>
     <t>Count of fish corresponding to est_cg reported in interview</t>
   </si>
   <si>
@@ -301,9 +266,6 @@
     <t>period</t>
   </si>
   <si>
-    <t>DayType</t>
-  </si>
-  <si>
     <t>n_obs</t>
   </si>
   <si>
@@ -337,9 +299,6 @@
     <t>section</t>
   </si>
   <si>
-    <t xml:space="preserve">Specification of the spatial domain used to aggregate observations from individual survey locations. A section contains one or more sites where effort counts and interviews occur. </t>
-  </si>
-  <si>
     <t>each fishery project specifies the sites and corresponding sections which define the fishery area</t>
   </si>
   <si>
@@ -370,25 +329,307 @@
     <t>Variance the stratum estimate</t>
   </si>
   <si>
-    <t>lower 95% confidence interval using the student t distribution</t>
-  </si>
-  <si>
-    <t>upper 95% confidence interval using the student t distribution</t>
-  </si>
-  <si>
     <t>catch_est_mean</t>
   </si>
   <si>
     <t>catch_est_var</t>
   </si>
   <si>
-    <t>categorical value for corresponding catch group to which estimate is associated</t>
-  </si>
-  <si>
     <t>Daily mean catch (count of fish) from observed days within a straum (sample mean)</t>
   </si>
   <si>
     <t>The expanded estimate of catch for the stratum, where catch_est_mean is multiplied by N_days_open</t>
+  </si>
+  <si>
+    <t>Specification of the spatial domain used to aggregate observations from individual survey locations; a section contains one or more sites where effort counts and interviews occur</t>
+  </si>
+  <si>
+    <t>Specification designating method used to count anglers during census surveys, either counting the total number of people in angler groups ("group") or counting only people observed actively fishing ("angler")</t>
+  </si>
+  <si>
+    <t>Directory name in file path where output from script is saved</t>
+  </si>
+  <si>
+    <t>Character string representing catch group of interest specified in the YAML metadata of the script</t>
+  </si>
+  <si>
+    <t>Boolean value determining if the angler group was interviewed by a WDFW creel sampler earlier in the day</t>
+  </si>
+  <si>
+    <t>Lower 95% confidence interval using the student t distribution</t>
+  </si>
+  <si>
+    <t>Upper 95% confidence interval using the student t distribution</t>
+  </si>
+  <si>
+    <t>Categorical value for corresponding catch group to which estimate is associated</t>
+  </si>
+  <si>
+    <t>input_options</t>
+  </si>
+  <si>
+    <t>"2022-12-15"</t>
+  </si>
+  <si>
+    <t>"2023-03-15"</t>
+  </si>
+  <si>
+    <t>"Naselle winter steelhead 2022-23"</t>
+  </si>
+  <si>
+    <t>Specification of one or more fish catch groups as a concatenation of strings using the fields: species, life_stage, fin_mark, and fate. Users can use "OR" operator  in R syntax (|) to aggregate groups within each of the four fields</t>
+  </si>
+  <si>
+    <t>Minimum date of observations fetched from data.wa.gov using format "yyyy-mm-dd"</t>
+  </si>
+  <si>
+    <t>Maximum date of observaitons fetched from data.wa.gov using format "yyyy-mm-dd"</t>
+  </si>
+  <si>
+    <t>"group"</t>
+  </si>
+  <si>
+    <t>"week"</t>
+  </si>
+  <si>
+    <t>"day"</t>
+  </si>
+  <si>
+    <t>c('Saturday', 'Sunday')</t>
+  </si>
+  <si>
+    <t>c(species = 'steelhead', life_stage = 'Adult', fin_mark = 'UM|AD', fate = 'Released')</t>
+  </si>
+  <si>
+    <t>"Vehicles/Trailers Only"</t>
+  </si>
+  <si>
+    <t>"Direct"</t>
+  </si>
+  <si>
+    <t>"model_output"</t>
+  </si>
+  <si>
+    <t>example_input</t>
+  </si>
+  <si>
+    <t>angler</t>
+  </si>
+  <si>
+    <t>group</t>
+  </si>
+  <si>
+    <t>week</t>
+  </si>
+  <si>
+    <t>month</t>
+  </si>
+  <si>
+    <t>duration</t>
+  </si>
+  <si>
+    <t>daily</t>
+  </si>
+  <si>
+    <t>Vehicle Only/Trailers Only</t>
+  </si>
+  <si>
+    <t>Bank Angler/Boat Angler</t>
+  </si>
+  <si>
+    <t>Direct</t>
+  </si>
+  <si>
+    <t>Indirect</t>
+  </si>
+  <si>
+    <t>parameter_options</t>
+  </si>
+  <si>
+    <t>"angler", "group"</t>
+  </si>
+  <si>
+    <t>"week", "month", "duration"</t>
+  </si>
+  <si>
+    <t>"day", "week"</t>
+  </si>
+  <si>
+    <t>Character string with naming convention "area season species year"</t>
+  </si>
+  <si>
+    <t>Character string with convention "species_lifestage_finmark_fate"</t>
+  </si>
+  <si>
+    <t>concatenation of character strings with convention 'name of day"</t>
+  </si>
+  <si>
+    <t>"Vehicles/Trailers Only", "Bank Angler/Boat Angler"</t>
+  </si>
+  <si>
+    <t>"Direct", "Indirect"</t>
+  </si>
+  <si>
+    <t>numeric value in hours</t>
+  </si>
+  <si>
+    <t>Character string identifying relative file path name</t>
+  </si>
+  <si>
+    <t>Time period for aggregation of observations for use in PE analysis</t>
+  </si>
+  <si>
+    <t>Time period for aggregation of observations for use in BSS analysis</t>
+  </si>
+  <si>
+    <t>The objects or anglers that are counted during index effort counts, either "Vehicle/Trailers Only" or "Bank Angler / Boat Angler"</t>
+  </si>
+  <si>
+    <t>Control option to use either observed census data ("Direct") or assumed values ("Indirect") to calculate the effort bias term ratio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Character string with waterbody area, focal species, year / year-group used to fetch a subset of data for analysis </t>
+  </si>
+  <si>
+    <t>Filter value for the minimum fishing time per angler group interview; used to remove short-duration interviews from the analysis</t>
+  </si>
+  <si>
+    <t>Days, Monday through Sunday, assigned to "weekend" day type; days not specified default to "weekday" day type</t>
+  </si>
+  <si>
+    <t>day</t>
+  </si>
+  <si>
+    <t>day_type</t>
+  </si>
+  <si>
+    <t>day_type_num</t>
+  </si>
+  <si>
+    <t>day_length</t>
+  </si>
+  <si>
+    <t>day_index</t>
+  </si>
+  <si>
+    <t>week_index</t>
+  </si>
+  <si>
+    <t>month_index</t>
+  </si>
+  <si>
+    <t>open_section_n</t>
+  </si>
+  <si>
+    <t>Date of the week, Monday:Sunday</t>
+  </si>
+  <si>
+    <t>Categorical designation of days of the week, either "weekend" or "weekday"</t>
+  </si>
+  <si>
+    <t>Index value of day_type with 0 = weekday, 1 = weekend</t>
+  </si>
+  <si>
+    <t xml:space="preserve">duration in hours of daylight from </t>
+  </si>
+  <si>
+    <t>%W format option for week, aggregating days into weeks numbering  00-53 with Monday as first day of the week</t>
+  </si>
+  <si>
+    <t>%m format option for month, aggregating days into months numbering  01-12</t>
+  </si>
+  <si>
+    <t>Time period used for temporal stratification of angler effort and catch estimates</t>
+  </si>
+  <si>
+    <t>Index value of event_date field</t>
+  </si>
+  <si>
+    <t>Index value of week field</t>
+  </si>
+  <si>
+    <t>Index value of month field</t>
+  </si>
+  <si>
+    <t>boolean (TRUE/FALSE) indicating if a section was open for fishing with a column for each section within with the fishery</t>
+  </si>
+  <si>
+    <t>angler_hours_daily_mean</t>
+  </si>
+  <si>
+    <t>TI_expan_final</t>
+  </si>
+  <si>
+    <t>ang_hrs_daily_mean_TI_expan</t>
+  </si>
+  <si>
+    <t>Stratum sample mean of effort (angler hours) without bias term ratio</t>
+  </si>
+  <si>
+    <t>Stratum sample mean of effort (angler hours) multipled by bias term ratio</t>
+  </si>
+  <si>
+    <t>ang_per_vhcl_trlr</t>
+  </si>
+  <si>
+    <t>Categorical assignment of angler type</t>
+  </si>
+  <si>
+    <t>Bias term ratio; cumulative sum of anglers from census counts divided by cumulative sum of anglers from index counts</t>
+  </si>
+  <si>
+    <t>Ratio representing the cumulative sum of the field person_count_final divided by the cumulative sum of the vehicle_count and trailer_count, from dwg_summarized_interview</t>
+  </si>
+  <si>
+    <t>p_census</t>
+  </si>
+  <si>
+    <t>census_indir</t>
+  </si>
+  <si>
+    <t>cen_exp_meth</t>
+  </si>
+  <si>
+    <t>Estimated proportion of a section that is surveyable during census counts; 1 indicates an entire section is surveyable</t>
+  </si>
+  <si>
+    <t>Default value for the bias term ratio when the parameter census_expansion is "Indirect"</t>
+  </si>
+  <si>
+    <t>Control option set from parameter census_expansion, "Direct" uses an observed ratio of census to index counts and "Indirect" uses an assumed value from the field census_indir</t>
+  </si>
+  <si>
+    <t>Index value for the section of a stratum estimate</t>
+  </si>
+  <si>
+    <t>Index value for the time period of a stratum estimate</t>
+  </si>
+  <si>
+    <t>The number of days that a section was open stratified by period, day_type, and section_num</t>
+  </si>
+  <si>
+    <t>n_days_samp</t>
+  </si>
+  <si>
+    <t>The number of days that a section was surveyed stratified by period, day_type, and section_num</t>
+  </si>
+  <si>
+    <t>Degrees of freedom stratified by section_num and angler_final; only applicable to "duration" option of paramter period_pe</t>
+  </si>
+  <si>
+    <t>index count type</t>
+  </si>
+  <si>
+    <t>effort count event</t>
+  </si>
+  <si>
+    <t>Categorical assignment of the objects being counted during index effort counts</t>
+  </si>
+  <si>
+    <t>Vehicle Only, Trailers Only, Bank Angler, Boat Angler</t>
+  </si>
+  <si>
+    <t>Temporal grouping of index effort counts associated with a scheduled count</t>
   </si>
 </sst>
 </file>
@@ -437,7 +678,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -447,6 +688,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -761,10 +1008,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8884888-2887-40E7-9CF4-425C1A207D31}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B17:B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -776,62 +1023,600 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="B1" t="s">
         <v>9</v>
       </c>
       <c r="C1" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="B2" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="C2" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="B3" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="C3" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="B4" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="C4" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B5" t="s">
         <v>97</v>
       </c>
-      <c r="B5" t="s">
-        <v>98</v>
-      </c>
       <c r="C5" t="s">
-        <v>99</v>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>189</v>
+      </c>
+      <c r="B6" t="s">
+        <v>191</v>
+      </c>
+      <c r="C6" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>190</v>
+      </c>
+      <c r="B7" t="s">
+        <v>193</v>
+      </c>
+      <c r="C7" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27751C24-16F2-45D7-AE42-E8195D4EC583}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.28515625" customWidth="1"/>
+    <col min="2" max="2" width="159.7109375" customWidth="1"/>
+    <col min="3" max="3" width="125.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>173</v>
+      </c>
+      <c r="B3" t="s">
+        <v>176</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA05063D-04D9-4A0D-966D-B047C181B015}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.28515625" customWidth="1"/>
+    <col min="2" max="2" width="161.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>177</v>
+      </c>
+      <c r="B4" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>178</v>
+      </c>
+      <c r="B5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>179</v>
+      </c>
+      <c r="B6" t="s">
+        <v>182</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43240694-B200-41EA-88D6-4BD59FC816F9}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.85546875" customWidth="1"/>
+    <col min="2" max="2" width="89.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>150</v>
+      </c>
+      <c r="B3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B5" t="s">
+        <v>185</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6913BFB8-E058-4A52-8E89-1CD515BF24AF}">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B19" sqref="B18:B19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.7109375" customWidth="1"/>
+    <col min="2" max="2" width="114" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>150</v>
+      </c>
+      <c r="B4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>186</v>
+      </c>
+      <c r="B6" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>76</v>
+      </c>
+      <c r="B7" t="s">
+        <v>188</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A75E7F5D-D201-4287-A106-3CF707809EE2}">
+  <dimension ref="A1:B14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.42578125" customWidth="1"/>
+    <col min="2" max="2" width="147.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B3" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>150</v>
+      </c>
+      <c r="B4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B6" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>73</v>
+      </c>
+      <c r="B7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>74</v>
+      </c>
+      <c r="B8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>75</v>
+      </c>
+      <c r="B9" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>76</v>
+      </c>
+      <c r="B10" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>77</v>
+      </c>
+      <c r="B11" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>78</v>
+      </c>
+      <c r="B12" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>79</v>
+      </c>
+      <c r="B13" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>80</v>
+      </c>
+      <c r="B14" t="s">
+        <v>103</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA93150C-F2EF-4B20-BF9C-B8E1EA328C72}">
+  <dimension ref="A1:B15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20" customWidth="1"/>
+    <col min="2" max="2" width="138.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B3" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>150</v>
+      </c>
+      <c r="B4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B7" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>93</v>
+      </c>
+      <c r="B8" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>94</v>
+      </c>
+      <c r="B9" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>75</v>
+      </c>
+      <c r="B10" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>76</v>
+      </c>
+      <c r="B11" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>77</v>
+      </c>
+      <c r="B12" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>78</v>
+      </c>
+      <c r="B13" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>79</v>
+      </c>
+      <c r="B14" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>80</v>
+      </c>
+      <c r="B15" t="s">
+        <v>103</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -840,12 +1625,14 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="9.140625" style="1"/>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="130" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="1"/>
     <col min="4" max="4" width="19.28515625" style="1" customWidth="1"/>
     <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
@@ -919,123 +1706,201 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C534D12-2EFF-44CC-BEBB-F36901043652}">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.28515625" customWidth="1"/>
-    <col min="2" max="2" width="94.5703125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="14" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="62.42578125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="52.140625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="104.28515625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>8</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+        <v>136</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>14</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>15</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>16</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>17</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="B10" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>19</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>20</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+      <c r="C12" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>21</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>33</v>
+        <v>141</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -1045,11 +1910,126 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A894F4F2-2062-48A4-8EB9-B058EC4938B2}">
+  <dimension ref="A1:B12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.7109375" customWidth="1"/>
+    <col min="2" max="2" width="31" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" t="s">
+        <v>130</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A04E9AE-1056-4C2D-948C-5977BC825BBB}">
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1060,7 +2040,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="B1" t="s">
         <v>9</v>
@@ -1068,130 +2048,130 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="B3" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="B4" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="B5" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="B6" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="B7" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="B8" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="B9" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="B10" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="B11" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="B12" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="B13" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="B14" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="B15" t="s">
-        <v>63</v>
+        <v>101</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="B16" t="s">
-        <v>64</v>
+        <v>100</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="B17" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1200,12 +2180,136 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26B19FED-B646-44AC-AB7F-C842D2973682}">
+  <dimension ref="A1:B13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19" customWidth="1"/>
+    <col min="2" max="2" width="109.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>149</v>
+      </c>
+      <c r="B3" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>150</v>
+      </c>
+      <c r="B4" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>151</v>
+      </c>
+      <c r="B5" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>152</v>
+      </c>
+      <c r="B6" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>123</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>124</v>
+      </c>
+      <c r="B8" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>71</v>
+      </c>
+      <c r="B9" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>153</v>
+      </c>
+      <c r="B10" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>154</v>
+      </c>
+      <c r="B11" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>155</v>
+      </c>
+      <c r="B12" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>156</v>
+      </c>
+      <c r="B13" t="s">
+        <v>167</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67FD1DF6-7FC0-408B-AD62-D1ECD6AEDCDF}">
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1216,7 +2320,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="B1" t="s">
         <v>9</v>
@@ -1224,42 +2328,42 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="B3" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4" t="s">
         <v>66</v>
-      </c>
-      <c r="B4" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" t="s">
         <v>67</v>
-      </c>
-      <c r="B5" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6" t="s">
         <v>68</v>
-      </c>
-      <c r="B6" t="s">
-        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -1268,12 +2372,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12605542-A2C1-4215-B756-E02144100F73}">
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1284,7 +2388,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="B1" t="s">
         <v>9</v>
@@ -1292,58 +2396,58 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="B3" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" t="s">
         <v>69</v>
-      </c>
-      <c r="B4" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" t="s">
         <v>66</v>
-      </c>
-      <c r="B5" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="B6" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="B7" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B8" t="s">
         <v>70</v>
-      </c>
-      <c r="B8" t="s">
-        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -1352,23 +2456,23 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A75E7F5D-D201-4287-A106-3CF707809EE2}">
-  <dimension ref="A1:B14"/>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70C7A05B-663B-4989-924A-8092E62B7888}">
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B14"/>
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.42578125" customWidth="1"/>
-    <col min="2" max="2" width="147.42578125" customWidth="1"/>
+    <col min="1" max="1" width="44.5703125" customWidth="1"/>
+    <col min="2" max="2" width="106.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="B1" t="s">
         <v>9</v>
@@ -1376,246 +2480,58 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>85</v>
+        <v>150</v>
       </c>
       <c r="B3" t="s">
-        <v>102</v>
+        <v>158</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>86</v>
+        <v>25</v>
       </c>
       <c r="B4" t="s">
-        <v>100</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="B5" t="s">
-        <v>53</v>
+        <v>174</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>87</v>
+        <v>168</v>
       </c>
       <c r="B6" t="s">
-        <v>101</v>
+        <v>171</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>88</v>
+        <v>169</v>
       </c>
       <c r="B7" t="s">
-        <v>103</v>
+        <v>175</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>89</v>
+        <v>170</v>
       </c>
       <c r="B8" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>90</v>
-      </c>
-      <c r="B9" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>91</v>
-      </c>
-      <c r="B10" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>92</v>
-      </c>
-      <c r="B11" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>93</v>
-      </c>
-      <c r="B12" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>94</v>
-      </c>
-      <c r="B13" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>95</v>
-      </c>
-      <c r="B14" t="s">
-        <v>110</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA93150C-F2EF-4B20-BF9C-B8E1EA328C72}">
-  <dimension ref="A1:B15"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="20" customWidth="1"/>
-    <col min="2" max="2" width="138.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B2" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>85</v>
-      </c>
-      <c r="B3" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>86</v>
-      </c>
-      <c r="B4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>49</v>
-      </c>
-      <c r="B6" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>87</v>
-      </c>
-      <c r="B7" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>111</v>
-      </c>
-      <c r="B8" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>112</v>
-      </c>
-      <c r="B9" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>90</v>
-      </c>
-      <c r="B10" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>91</v>
-      </c>
-      <c r="B11" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>92</v>
-      </c>
-      <c r="B12" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>93</v>
-      </c>
-      <c r="B13" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>94</v>
-      </c>
-      <c r="B14" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>95</v>
-      </c>
-      <c r="B15" t="s">
-        <v>110</v>
+        <v>172</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
small cleanup and setting fishery_name to Nisqually salmon 2022 in fw_creel.Rmd and establish_analysis.R
adding folder project_scripts

Updated documentation files
</commit_message>
<xml_diff>
--- a/documentation_files/documentation_tables.xlsx
+++ b/documentation_files/documentation_tables.xlsx
@@ -8,26 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stateofwa-my.sharepoint.com/personal/evan_booher_dfw_wa_gov/Documents/code/CreelEstimates/documentation_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="531" documentId="13_ncr:1_{06BDCB52-A10A-4652-9501-BAA58E581D65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9D10B5A8-E911-4088-83E0-CDB5A159C6B8}"/>
+  <xr:revisionPtr revIDLastSave="594" documentId="13_ncr:1_{06BDCB52-A10A-4652-9501-BAA58E581D65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{302421DA-0B90-4B17-BB60-8A31AA26AC16}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D87A213F-20EA-453F-96F1-E2F9D588DE08}"/>
+    <workbookView xWindow="2580" yWindow="1680" windowWidth="25560" windowHeight="13050" firstSheet="1" activeTab="4" xr2:uid="{D87A213F-20EA-453F-96F1-E2F9D588DE08}"/>
   </bookViews>
   <sheets>
     <sheet name="design_stratification" sheetId="7" r:id="rId1"/>
     <sheet name="pre_analysis_checklist" sheetId="1" r:id="rId2"/>
     <sheet name="YAML_parameters" sheetId="2" r:id="rId3"/>
     <sheet name="YAML_param_options" sheetId="9" r:id="rId4"/>
-    <sheet name="dwg_summ_interview" sheetId="4" r:id="rId5"/>
-    <sheet name="fetch_days_output" sheetId="10" r:id="rId6"/>
-    <sheet name="dwg_summ_effort_index" sheetId="6" r:id="rId7"/>
-    <sheet name="dwg_summ_effort_census" sheetId="5" r:id="rId8"/>
-    <sheet name="inputs_pe_ang_hours_daily_mean" sheetId="11" r:id="rId9"/>
-    <sheet name="inputs_pe$angler_per_vehicle_tr" sheetId="12" r:id="rId10"/>
-    <sheet name="inputs_pe$census" sheetId="13" r:id="rId11"/>
-    <sheet name="inputs_pe$days_total" sheetId="14" r:id="rId12"/>
-    <sheet name="inputs_pe$df" sheetId="15" r:id="rId13"/>
-    <sheet name="PE_effort" sheetId="3" r:id="rId14"/>
-    <sheet name="PE_catch" sheetId="8" r:id="rId15"/>
+    <sheet name="creel_fishery_lut" sheetId="17" r:id="rId5"/>
+    <sheet name="dwg_summ_interview" sheetId="4" r:id="rId6"/>
+    <sheet name="fetch_days_output" sheetId="10" r:id="rId7"/>
+    <sheet name="dwg_summ_effort_index" sheetId="6" r:id="rId8"/>
+    <sheet name="dwg_summ_effort_census" sheetId="5" r:id="rId9"/>
+    <sheet name="inputs_pe_ang_hours_daily_mean" sheetId="11" r:id="rId10"/>
+    <sheet name="inputs_pe$angler_per_vehicle_tr" sheetId="12" r:id="rId11"/>
+    <sheet name="inputs_pe$census" sheetId="13" r:id="rId12"/>
+    <sheet name="inputs_pe$days_total" sheetId="14" r:id="rId13"/>
+    <sheet name="inputs_pe$df" sheetId="15" r:id="rId14"/>
+    <sheet name="PE_effort" sheetId="3" r:id="rId15"/>
+    <sheet name="PE_catch" sheetId="8" r:id="rId16"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -48,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="258">
   <si>
     <t>Data is stored in the creel database and accessible from data.wa.gov</t>
   </si>
@@ -113,9 +114,6 @@
     <t>min_fishing_time</t>
   </si>
   <si>
-    <t>dir_output</t>
-  </si>
-  <si>
     <t>field</t>
   </si>
   <si>
@@ -227,18 +225,12 @@
     <t>options</t>
   </si>
   <si>
-    <t>Categorical assignment of the angler effort and catch based on a combinaton of observed fishing location and reported means to access the fishery area</t>
-  </si>
-  <si>
     <t>weekday, weekend</t>
   </si>
   <si>
     <t>bank, boat</t>
   </si>
   <si>
-    <t>Specification of variable used to group n days of observations</t>
-  </si>
-  <si>
     <t>varies by estimation method; daily, week, month, "duration"</t>
   </si>
   <si>
@@ -335,15 +327,9 @@
     <t>The expanded estimate of catch for the stratum, where catch_est_mean is multiplied by N_days_open</t>
   </si>
   <si>
-    <t>Specification of the spatial domain used to aggregate observations from individual survey locations; a section contains one or more sites where effort counts and interviews occur</t>
-  </si>
-  <si>
     <t>Specification designating method used to count anglers during census surveys, either counting the total number of people in angler groups ("group") or counting only people observed actively fishing ("angler")</t>
   </si>
   <si>
-    <t>Directory name in file path where output from script is saved</t>
-  </si>
-  <si>
     <t>Character string representing catch group of interest specified in the YAML metadata of the script</t>
   </si>
   <si>
@@ -401,9 +387,6 @@
     <t>"Direct"</t>
   </si>
   <si>
-    <t>"model_output"</t>
-  </si>
-  <si>
     <t>example_input</t>
   </si>
   <si>
@@ -467,9 +450,6 @@
     <t>numeric value in hours</t>
   </si>
   <si>
-    <t>Character string identifying relative file path name</t>
-  </si>
-  <si>
     <t>Time period for aggregation of observations for use in PE analysis</t>
   </si>
   <si>
@@ -626,9 +606,6 @@
     <t>Temporal grouping of index effort counts associated with a scheduled count</t>
   </si>
   <si>
-    <t>formula_variable</t>
-  </si>
-  <si>
     <t>day-type</t>
   </si>
   <si>
@@ -645,13 +622,217 @@
   </si>
   <si>
     <t xml:space="preserve">Sample unit encompassing the trip information collected from a complete interview with an angler group </t>
+  </si>
+  <si>
+    <t>Specification of the “day type” used to aggregate n days within a week</t>
+  </si>
+  <si>
+    <t>Specification of the time step used to aggregate n days of observations from creel surveys</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Specification of the spatial domain used to aggregate observations from individual survey locations. A section contains one or more sites where effort counts and interviews occur. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Categorical assignment of the angler effort and catch based on a combinaton of observed fishing location and reported method used to access the fishery area </t>
+  </si>
+  <si>
+    <t>angler groups are either defined as the total group size (default) or the total angler count</t>
+  </si>
+  <si>
+    <t>project_name</t>
+  </si>
+  <si>
+    <t>"District 17 North"</t>
+  </si>
+  <si>
+    <t>Character string with naming covention matching work unit</t>
+  </si>
+  <si>
+    <t>Grouping variable used to define work unit that manages a give fishery_name</t>
+  </si>
+  <si>
+    <t>output_location_filepath</t>
+  </si>
+  <si>
+    <t>local</t>
+  </si>
+  <si>
+    <t>teams</t>
+  </si>
+  <si>
+    <t>output_teams_name</t>
+  </si>
+  <si>
+    <t>"DFW-Team FP FW Creel Monitoring Program - General"</t>
+  </si>
+  <si>
+    <t>if "teams" used for output_location_filepath, the character string identifying teams folder where output is saved</t>
+  </si>
+  <si>
+    <t>character string matching name of teams folder</t>
+  </si>
+  <si>
+    <t>"local", "teams"</t>
+  </si>
+  <si>
+    <t>"teams"</t>
+  </si>
+  <si>
+    <t>variable used to route output to either the project_outputs folder (local) or a shared network drive location (teams)</t>
+  </si>
+  <si>
+    <t>District 17 South</t>
+  </si>
+  <si>
+    <t>District 13</t>
+  </si>
+  <si>
+    <t>District 14</t>
+  </si>
+  <si>
+    <t>District 16</t>
+  </si>
+  <si>
+    <t>Cowlitz</t>
+  </si>
+  <si>
+    <t>District 17 North</t>
+  </si>
+  <si>
+    <t>District 11</t>
+  </si>
+  <si>
+    <t>R5 Steelhead</t>
+  </si>
+  <si>
+    <t>fishery_start_date</t>
+  </si>
+  <si>
+    <t>fishery_end_date</t>
+  </si>
+  <si>
+    <t>Skagit fall salmon 2021</t>
+  </si>
+  <si>
+    <t>Baker summer sockeye 2022</t>
+  </si>
+  <si>
+    <t>Naselle winter steelhead 2022</t>
+  </si>
+  <si>
+    <t>Nooksack spring Chinook 2022</t>
+  </si>
+  <si>
+    <t>Skagit spring Chinook 2021 upper</t>
+  </si>
+  <si>
+    <t>Skagit spring Chinook 2022 upper</t>
+  </si>
+  <si>
+    <t>Skagit spring Chinook 2022 lower</t>
+  </si>
+  <si>
+    <t>Skykomish summer Chinook 2021</t>
+  </si>
+  <si>
+    <t>Willapa winter steelhead 2022</t>
+  </si>
+  <si>
+    <t>Nisqually salmon 2022</t>
+  </si>
+  <si>
+    <t>Puyallup_Carbon salmon 2022</t>
+  </si>
+  <si>
+    <t>Skagit summer gamefish 2022</t>
+  </si>
+  <si>
+    <t>Quillayute fall salmon 2022</t>
+  </si>
+  <si>
+    <t>Skagit summer sockeye 2022</t>
+  </si>
+  <si>
+    <t>Skykomish winter gamefish 2021-22</t>
+  </si>
+  <si>
+    <t>Stillaguamish salmon and gamefish 2022-23</t>
+  </si>
+  <si>
+    <t>Skagit winter steelhead 2021</t>
+  </si>
+  <si>
+    <t>Skykomish summer Chinook and gamefish 2022</t>
+  </si>
+  <si>
+    <t>Wallace salmon and gamefish 2022-23</t>
+  </si>
+  <si>
+    <t>Cascade fall salmon 2022</t>
+  </si>
+  <si>
+    <t>Skagit fall salmon 2022</t>
+  </si>
+  <si>
+    <t>Cascade fall salmon 2021</t>
+  </si>
+  <si>
+    <t>Cascade spring Chinook 2021</t>
+  </si>
+  <si>
+    <t>Cascade spring Chinook 2022</t>
+  </si>
+  <si>
+    <t>Snoqualmie winter steelhead 2022-23</t>
+  </si>
+  <si>
+    <t>Nooksack winter gamefish 2022-23</t>
+  </si>
+  <si>
+    <t>Skagit winter gamefish 2022-23</t>
+  </si>
+  <si>
+    <t>Cascade winter gamefish 2021-22</t>
+  </si>
+  <si>
+    <t>Nooksack winter gamefish 2021-22</t>
+  </si>
+  <si>
+    <t>Skagit winter gamefish 2021-22</t>
+  </si>
+  <si>
+    <t>Willapa winter steelhead 2022-23</t>
+  </si>
+  <si>
+    <t>Naselle winter steelhead 2022-23</t>
+  </si>
+  <si>
+    <t>Satsop salmon 2022</t>
+  </si>
+  <si>
+    <t>Humptulips salmon 2022</t>
+  </si>
+  <si>
+    <t>Chehalis salmon 2022</t>
+  </si>
+  <si>
+    <t>Hoh winter steelhead 2022-23</t>
+  </si>
+  <si>
+    <t>Cascade winter gamefish 2023</t>
+  </si>
+  <si>
+    <t>Skagit winter steelhead 2023</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -672,6 +853,17 @@
       <name val="Source Sans Pro"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -681,7 +873,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -689,11 +881,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="22"/>
+      </left>
+      <right style="thin">
+        <color indexed="22"/>
+      </right>
+      <top style="thin">
+        <color indexed="22"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="22"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -709,9 +917,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal_Sheet1" xfId="1" xr:uid="{2D0D78B3-5B15-4E1E-BC8A-A19FCA854AE2}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1023,116 +1235,116 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8884888-2887-40E7-9CF4-425C1A207D31}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D15:D16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M15" sqref="M15:M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="21" customWidth="1"/>
-    <col min="3" max="3" width="160.42578125" customWidth="1"/>
-    <col min="4" max="4" width="91.5703125" customWidth="1"/>
+    <col min="1" max="1" width="21" customWidth="1"/>
+    <col min="2" max="2" width="160.42578125" customWidth="1"/>
+    <col min="3" max="3" width="91.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" t="s">
         <v>192</v>
       </c>
-      <c r="C1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="C2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>185</v>
+      </c>
+      <c r="B3" t="s">
+        <v>191</v>
+      </c>
+      <c r="C3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C2" t="s">
-        <v>62</v>
-      </c>
-      <c r="D2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>193</v>
-      </c>
-      <c r="C3" t="s">
-        <v>82</v>
-      </c>
-      <c r="D3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>186</v>
+      </c>
+      <c r="B4" t="s">
         <v>194</v>
       </c>
       <c r="C4" t="s">
         <v>59</v>
       </c>
-      <c r="D4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>80</v>
+        <v>77</v>
+      </c>
+      <c r="B5" t="s">
+        <v>193</v>
       </c>
       <c r="C5" t="s">
-        <v>95</v>
-      </c>
-      <c r="D5" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>180</v>
+      </c>
+      <c r="B6" t="s">
+        <v>182</v>
+      </c>
+      <c r="C6" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>181</v>
+      </c>
+      <c r="B7" t="s">
+        <v>184</v>
+      </c>
+      <c r="C7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>181</v>
+      </c>
+      <c r="B8" t="s">
         <v>187</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C8" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>189</v>
       </c>
-      <c r="D6" t="s">
+      <c r="B9" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>188</v>
-      </c>
-      <c r="C7" t="s">
-        <v>191</v>
-      </c>
-      <c r="D7" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>188</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="C9" t="s">
         <v>195</v>
-      </c>
-      <c r="D8" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>197</v>
-      </c>
-      <c r="C9" t="s">
-        <v>198</v>
       </c>
     </row>
   </sheetData>
@@ -1142,6 +1354,89 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70C7A05B-663B-4989-924A-8092E62B7888}">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="44.5703125" customWidth="1"/>
+    <col min="2" max="2" width="106.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>141</v>
+      </c>
+      <c r="B3" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>159</v>
+      </c>
+      <c r="B6" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>160</v>
+      </c>
+      <c r="B7" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>161</v>
+      </c>
+      <c r="B8" t="s">
+        <v>163</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27751C24-16F2-45D7-AE42-E8195D4EC583}">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -1158,7 +1453,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
         <v>9</v>
@@ -1166,18 +1461,18 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="B3" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
     </row>
   </sheetData>
@@ -1185,7 +1480,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA05063D-04D9-4A0D-966D-B047C181B015}">
   <dimension ref="A1:B6"/>
   <sheetViews>
@@ -1201,7 +1496,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
         <v>9</v>
@@ -1209,42 +1504,42 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B3" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="B4" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="B5" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="B6" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
     </row>
   </sheetData>
@@ -1252,7 +1547,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43240694-B200-41EA-88D6-4BD59FC816F9}">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -1268,7 +1563,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
         <v>9</v>
@@ -1276,34 +1571,34 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="B3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B5" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
     </row>
   </sheetData>
@@ -1311,7 +1606,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6913BFB8-E058-4A52-8E89-1CD515BF24AF}">
   <dimension ref="A1:B7"/>
   <sheetViews>
@@ -1327,7 +1622,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
         <v>9</v>
@@ -1335,50 +1630,50 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="B4" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="B6" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B7" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
     </row>
   </sheetData>
@@ -1386,7 +1681,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A75E7F5D-D201-4287-A106-3CF707809EE2}">
   <dimension ref="A1:B14"/>
   <sheetViews>
@@ -1402,7 +1697,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
         <v>9</v>
@@ -1410,106 +1705,106 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B3" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="B4" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B6" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B7" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B8" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B9" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B10" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B11" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B12" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B13" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B14" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -1518,7 +1813,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA93150C-F2EF-4B20-BF9C-B8E1EA328C72}">
   <dimension ref="A1:B15"/>
   <sheetViews>
@@ -1534,7 +1829,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
         <v>9</v>
@@ -1542,114 +1837,114 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B3" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="B4" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B6" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B7" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B8" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B9" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B10" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B11" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B12" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B13" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B14" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B15" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -1743,15 +2038,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C534D12-2EFF-44CC-BEBB-F36901043652}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" customWidth="1"/>
+    <col min="1" max="1" width="24.42578125" customWidth="1"/>
     <col min="2" max="2" width="62.42578125" style="3" customWidth="1"/>
     <col min="3" max="3" width="52.140625" style="6" customWidth="1"/>
     <col min="4" max="4" width="104.28515625" style="3" customWidth="1"/>
@@ -1763,181 +2058,209 @@
         <v>8</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>196</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>11</v>
-      </c>
       <c r="B3" s="3" t="s">
-        <v>40</v>
+        <v>127</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>108</v>
+        <v>137</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C4" s="6" t="s">
+      <c r="B5" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C7" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>111</v>
-      </c>
       <c r="D7" s="3" t="s">
-        <v>140</v>
+        <v>92</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>17</v>
-      </c>
       <c r="B9" s="3" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>136</v>
+        <v>17</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>129</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>137</v>
+        <v>18</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>130</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B13" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="C13" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="C12" s="6">
-        <v>0.5</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>97</v>
+    </row>
+    <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>200</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>203</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>205</v>
       </c>
     </row>
   </sheetData>
@@ -1948,15 +2271,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A894F4F2-2062-48A4-8EB9-B058EC4938B2}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+      <selection activeCell="B11" sqref="A9:B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.7109375" customWidth="1"/>
+    <col min="1" max="1" width="25.7109375" customWidth="1"/>
     <col min="2" max="2" width="31" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1965,95 +2288,175 @@
         <v>8</v>
       </c>
       <c r="B1" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>196</v>
       </c>
       <c r="B2" t="s">
-        <v>119</v>
+        <v>210</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>196</v>
       </c>
       <c r="B3" t="s">
-        <v>120</v>
+        <v>211</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>196</v>
       </c>
       <c r="B4" t="s">
-        <v>121</v>
+        <v>212</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>196</v>
       </c>
       <c r="B5" t="s">
-        <v>122</v>
+        <v>213</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>196</v>
       </c>
       <c r="B6" t="s">
-        <v>123</v>
+        <v>214</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>196</v>
       </c>
       <c r="B7" t="s">
-        <v>124</v>
+        <v>215</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>196</v>
       </c>
       <c r="B8" t="s">
-        <v>121</v>
+        <v>216</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>196</v>
       </c>
       <c r="B9" t="s">
-        <v>125</v>
+        <v>217</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>19</v>
       </c>
-      <c r="B12" t="s">
-        <v>128</v>
+      <c r="B19" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>200</v>
+      </c>
+      <c r="B21" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>200</v>
+      </c>
+      <c r="B22" t="s">
+        <v>202</v>
       </c>
     </row>
   </sheetData>
@@ -2062,11 +2465,460 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16A05A0A-C7D1-40EE-9E15-74F73361602C}">
+  <dimension ref="A1:C39"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="45.7109375" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" customWidth="1"/>
+    <col min="3" max="3" width="18" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C1" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>220</v>
+      </c>
+      <c r="B2" s="7">
+        <v>44422</v>
+      </c>
+      <c r="C2" s="7">
+        <v>44561</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>221</v>
+      </c>
+      <c r="B3" s="7">
+        <v>44751</v>
+      </c>
+      <c r="C3" s="7">
+        <v>44804</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>222</v>
+      </c>
+      <c r="B4" s="7">
+        <v>44562</v>
+      </c>
+      <c r="C4" s="7">
+        <v>44620</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>223</v>
+      </c>
+      <c r="B5" s="7">
+        <v>44709</v>
+      </c>
+      <c r="C5" s="7">
+        <v>44752</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>224</v>
+      </c>
+      <c r="B6" s="7">
+        <v>44348</v>
+      </c>
+      <c r="C6" s="7">
+        <v>44392</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>225</v>
+      </c>
+      <c r="B7" s="7">
+        <v>44713</v>
+      </c>
+      <c r="C7" s="7">
+        <v>44757</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>226</v>
+      </c>
+      <c r="B8" s="7">
+        <v>44682</v>
+      </c>
+      <c r="C8" s="7">
+        <v>44712</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>227</v>
+      </c>
+      <c r="B9" s="7">
+        <v>44345</v>
+      </c>
+      <c r="C9" s="7">
+        <v>44395</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>228</v>
+      </c>
+      <c r="B10" s="7">
+        <v>44562</v>
+      </c>
+      <c r="C10" s="7">
+        <v>44620</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>229</v>
+      </c>
+      <c r="B11" s="7">
+        <v>44743</v>
+      </c>
+      <c r="C11" s="7">
+        <v>44880</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>230</v>
+      </c>
+      <c r="B12" s="7">
+        <v>44789</v>
+      </c>
+      <c r="C12" s="7">
+        <v>44834</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>231</v>
+      </c>
+      <c r="B13" s="7">
+        <v>44757</v>
+      </c>
+      <c r="C13" s="7">
+        <v>44804</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>232</v>
+      </c>
+      <c r="B14" s="7">
+        <v>44805</v>
+      </c>
+      <c r="C14" s="7">
+        <v>44910</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>233</v>
+      </c>
+      <c r="B15" s="7">
+        <v>44728</v>
+      </c>
+      <c r="C15" s="7">
+        <v>44771</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>234</v>
+      </c>
+      <c r="B16" s="7">
+        <v>44531</v>
+      </c>
+      <c r="C16" s="7">
+        <v>44607</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>235</v>
+      </c>
+      <c r="B17" s="7">
+        <v>44805</v>
+      </c>
+      <c r="C17" s="7">
+        <v>44957</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>236</v>
+      </c>
+      <c r="B18" s="7">
+        <v>44228</v>
+      </c>
+      <c r="C18" s="7">
+        <v>44301</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>237</v>
+      </c>
+      <c r="B19" s="7">
+        <v>44709</v>
+      </c>
+      <c r="C19" s="7">
+        <v>44804</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>238</v>
+      </c>
+      <c r="B20" s="7">
+        <v>44835</v>
+      </c>
+      <c r="C20" s="7">
+        <v>44972</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>239</v>
+      </c>
+      <c r="B21" s="7">
+        <v>44820</v>
+      </c>
+      <c r="C21" s="7">
+        <v>44895</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>240</v>
+      </c>
+      <c r="B22" s="7">
+        <v>44805</v>
+      </c>
+      <c r="C22" s="7">
+        <v>44895</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>241</v>
+      </c>
+      <c r="B23" s="7">
+        <v>44455</v>
+      </c>
+      <c r="C23" s="7">
+        <v>44530</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>242</v>
+      </c>
+      <c r="B24" s="7">
+        <v>44348</v>
+      </c>
+      <c r="C24" s="7">
+        <v>44392</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>243</v>
+      </c>
+      <c r="B25" s="7">
+        <v>44713</v>
+      </c>
+      <c r="C25" s="7">
+        <v>44757</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>244</v>
+      </c>
+      <c r="B26" s="7">
+        <v>44896</v>
+      </c>
+      <c r="C26" s="7">
+        <v>44972</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>245</v>
+      </c>
+      <c r="B27" s="7">
+        <v>44896</v>
+      </c>
+      <c r="C27" s="7">
+        <v>44972</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>246</v>
+      </c>
+      <c r="B28" s="7">
+        <v>44896</v>
+      </c>
+      <c r="C28" s="7">
+        <v>44957</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>247</v>
+      </c>
+      <c r="B29" s="7">
+        <v>44531</v>
+      </c>
+      <c r="C29" s="7">
+        <v>44592</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>248</v>
+      </c>
+      <c r="B30" s="7">
+        <v>44583</v>
+      </c>
+      <c r="C30" s="7">
+        <v>44607</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>249</v>
+      </c>
+      <c r="B31" s="7">
+        <v>44562</v>
+      </c>
+      <c r="C31" s="7">
+        <v>44592</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>250</v>
+      </c>
+      <c r="B32" s="7">
+        <v>44911</v>
+      </c>
+      <c r="C32" s="7">
+        <v>45016</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>251</v>
+      </c>
+      <c r="B33" s="7">
+        <v>44911</v>
+      </c>
+      <c r="C33" s="7">
+        <v>45016</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>252</v>
+      </c>
+      <c r="B34" s="7">
+        <v>44835</v>
+      </c>
+      <c r="C34" s="7">
+        <v>44911</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>253</v>
+      </c>
+      <c r="B35" s="7">
+        <v>44805</v>
+      </c>
+      <c r="C35" s="7">
+        <v>44911</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>254</v>
+      </c>
+      <c r="B36" s="7">
+        <v>44820</v>
+      </c>
+      <c r="C36" s="7">
+        <v>44911</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>255</v>
+      </c>
+      <c r="B37" s="7">
+        <v>44910</v>
+      </c>
+      <c r="C37" s="7">
+        <v>45016</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>256</v>
+      </c>
+      <c r="B38" s="7">
+        <v>44927</v>
+      </c>
+      <c r="C38" s="7">
+        <v>44957</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>257</v>
+      </c>
+      <c r="B39" s="7">
+        <v>44958</v>
+      </c>
+      <c r="C39" s="7">
+        <v>45031</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A04E9AE-1056-4C2D-948C-5977BC825BBB}">
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="A5" sqref="A5:A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2077,7 +2929,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
         <v>9</v>
@@ -2085,130 +2937,130 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B3" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B15" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B16" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -2217,7 +3069,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26B19FED-B646-44AC-AB7F-C842D2973682}">
   <dimension ref="A1:B13"/>
   <sheetViews>
@@ -2233,7 +3085,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
         <v>9</v>
@@ -2241,98 +3093,98 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="B3" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="B4" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="B5" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="B6" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="B8" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B9" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="B10" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="B11" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="B12" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="B13" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>
@@ -2341,7 +3193,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67FD1DF6-7FC0-408B-AD62-D1ECD6AEDCDF}">
   <dimension ref="A1:B6"/>
   <sheetViews>
@@ -2357,7 +3209,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
         <v>9</v>
@@ -2365,42 +3217,42 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B4" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B5" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -2409,7 +3261,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12605542-A2C1-4215-B756-E02144100F73}">
   <dimension ref="A1:B8"/>
   <sheetViews>
@@ -2425,7 +3277,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
         <v>9</v>
@@ -2433,145 +3285,62 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B4" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B8" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70C7A05B-663B-4989-924A-8092E62B7888}">
-  <dimension ref="A1:B8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="44.5703125" customWidth="1"/>
-    <col min="2" max="2" width="106.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>148</v>
-      </c>
-      <c r="B3" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B5" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>166</v>
-      </c>
-      <c r="B6" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>167</v>
-      </c>
-      <c r="B7" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>168</v>
-      </c>
-      <c r="B8" t="s">
-        <v>170</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
updated list and description of YAML parameters corresponding to updated R functions
</commit_message>
<xml_diff>
--- a/documentation_files/documentation_tables.xlsx
+++ b/documentation_files/documentation_tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stateofwa-my.sharepoint.com/personal/evan_booher_dfw_wa_gov/Documents/code/CreelEstimates/documentation_files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stateofwa-my.sharepoint.com/personal/kale_bentley_dfw_wa_gov/Documents/Projects/Creel/GitHub/CreelEstimates/documentation_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="594" documentId="13_ncr:1_{06BDCB52-A10A-4652-9501-BAA58E581D65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{302421DA-0B90-4B17-BB60-8A31AA26AC16}"/>
+  <xr:revisionPtr revIDLastSave="641" documentId="13_ncr:1_{06BDCB52-A10A-4652-9501-BAA58E581D65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AB3FD276-6CAC-4ACB-9FBD-845DE3387799}"/>
   <bookViews>
-    <workbookView xWindow="2580" yWindow="1680" windowWidth="25560" windowHeight="13050" firstSheet="1" activeTab="4" xr2:uid="{D87A213F-20EA-453F-96F1-E2F9D588DE08}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="2" xr2:uid="{D87A213F-20EA-453F-96F1-E2F9D588DE08}"/>
   </bookViews>
   <sheets>
     <sheet name="design_stratification" sheetId="7" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="273">
   <si>
     <t>Data is stored in the creel database and accessible from data.wa.gov</t>
   </si>
@@ -381,9 +381,6 @@
     <t>c(species = 'steelhead', life_stage = 'Adult', fin_mark = 'UM|AD', fate = 'Released')</t>
   </si>
   <si>
-    <t>"Vehicles/Trailers Only"</t>
-  </si>
-  <si>
     <t>"Direct"</t>
   </si>
   <si>
@@ -441,9 +438,6 @@
     <t>concatenation of character strings with convention 'name of day"</t>
   </si>
   <si>
-    <t>"Vehicles/Trailers Only", "Bank Angler/Boat Angler"</t>
-  </si>
-  <si>
     <t>"Direct", "Indirect"</t>
   </si>
   <si>
@@ -456,9 +450,6 @@
     <t>Time period for aggregation of observations for use in BSS analysis</t>
   </si>
   <si>
-    <t>The objects or anglers that are counted during index effort counts, either "Vehicle/Trailers Only" or "Bank Angler / Boat Angler"</t>
-  </si>
-  <si>
     <t>Control option to use either observed census data ("Direct") or assumed values ("Indirect") to calculate the effort bias term ratio</t>
   </si>
   <si>
@@ -823,6 +814,62 @@
   </si>
   <si>
     <t>Skagit winter steelhead 2023</t>
+  </si>
+  <si>
+    <t>study_design</t>
+  </si>
+  <si>
+    <t>boat_type_collapse</t>
+  </si>
+  <si>
+    <t>fish_location_determines_type</t>
+  </si>
+  <si>
+    <t>angler_type_kayak_pontoon</t>
+  </si>
+  <si>
+    <t>bss_model_file_name</t>
+  </si>
+  <si>
+    <t>"Standard", "Drano"</t>
+  </si>
+  <si>
+    <t>"Standard"</t>
+  </si>
+  <si>
+    <t>"Yes", "No"</t>
+  </si>
+  <si>
+    <t>"No"</t>
+  </si>
+  <si>
+    <t>Parameter/argument used in several prep_dwg_ and prep_inputs_pe_ functions denoting which study design was followed during data collection, which impacts how the data are wrangled and analyzed.  Currently, the CreelAnalysis scripts have updated to accommodate two approved study designs ("Standard", "Drano") such that estimates of effort and catch can be generated using both the PE and BSS models.</t>
+  </si>
+  <si>
+    <t>Parameter/argument used in several prep_dwg_ functions that controls whether a boat designated as a kayak, pontoon, or kick during an effort count or angler group interview should be designated as a boat or bank angler.</t>
+  </si>
+  <si>
+    <t>"bank", "boat"</t>
+  </si>
+  <si>
+    <t>"bank"</t>
+  </si>
+  <si>
+    <t>Parameter/argument used in several prep_dwg_ functions that controls whether all (potential) boat types (e.g., motor_boat, drift_boat) are collapsed (i.e., boat_type_collapse: "Yes") into a single boat type or kept separate (boat_type_collapse: "No").  If multiple boat types were enumerated/specified during effort counts and interviews, estimates of effort and catch can (and will) be generated for each unique boat type using the PE estimator if "boat_type_collapse" is set to "No".  However, the current version of the BSS model (updated in April 2024) only has two possible angler types (bank, boat).  Thus, to generate estimates using the BSS model, "boat_type_collapse" must be set to "Yes".</t>
+  </si>
+  <si>
+    <t>character string matching name of the desired BSS model contained within the "stan_models" folder</t>
+  </si>
+  <si>
+    <t>"BSS_creel_model_02_2024-04-03.stan"</t>
+  </si>
+  <si>
+    <t>parameter/argument used in the "fit_bss_dev" function when running/fitting a BSS model; 
+NOTE: data wrangling functions are designed to work with the most up-to-date model.  Therefore, the utility of this argument (i.e., having the ability to specify different BSS/stan models) may not be functional or needed.</t>
+  </si>
+  <si>
+    <t>Parameter/argument used in several prep_dwg_ functions that controls whether the observed fishing location for a given angler group during an effort count determines their angler type.  For instance, if fish_location_determines_type is set to Yes, a boat angler group observed fishing on the bank (i.e., their boat is pulled up on the bank) during an effort count would be designated as a bank angler in the analysis.  Conversely, if fish_location_determines_type is set to No, the angler type is determined by the presence/absence of a boat (i.e., watercraft) during the effort count regardless of where it was positioned during the effort count (i.e., a boat angler group is designated as a boat angler even if anglers were fishing from shore).  Similarly, this parameter/argument determines whether the field "fish_from_boat" (which is a field that is collected during interviews exclusively from boat anglers specifying where they spent the majority of the day fishing from: bank or boat) is used to determine the angler type.  If fish_location_determines_type is set to Yes then a boat angler interview can be designated as a bank angler is they reported fishing from the bank the majority of the day.  Conversely, if fish_location_determines_type is set to No then an angler group that has a boat during the interview will be designated as a boat angler regardless of how they responded to the "fish_from_boat" question.  
+NOTE: the "fish_from_boat" question/field is not asked in every creel.  Therefore, this argument can be deleted from the corresponding function is not appliable (the function will designate the argument as NA by default).</t>
   </si>
 </sst>
 </file>
@@ -830,7 +877,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -857,6 +904,7 @@
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -901,7 +949,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -912,12 +960,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1264,7 +1309,7 @@
         <v>56</v>
       </c>
       <c r="B2" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="C2" t="s">
         <v>60</v>
@@ -1272,10 +1317,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B3" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C3" t="s">
         <v>58</v>
@@ -1283,10 +1328,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B4" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C4" t="s">
         <v>59</v>
@@ -1297,7 +1342,7 @@
         <v>77</v>
       </c>
       <c r="B5" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="C5" t="s">
         <v>78</v>
@@ -1305,21 +1350,21 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>177</v>
+      </c>
+      <c r="B6" t="s">
+        <v>179</v>
+      </c>
+      <c r="C6" t="s">
         <v>180</v>
-      </c>
-      <c r="B6" t="s">
-        <v>182</v>
-      </c>
-      <c r="C6" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>178</v>
+      </c>
+      <c r="B7" t="s">
         <v>181</v>
-      </c>
-      <c r="B7" t="s">
-        <v>184</v>
       </c>
       <c r="C7" t="s">
         <v>51</v>
@@ -1327,24 +1372,24 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B8" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C8" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B9" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C9" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
   </sheetData>
@@ -1385,10 +1430,10 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B3" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1404,31 +1449,31 @@
         <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>156</v>
+      </c>
+      <c r="B6" t="s">
         <v>159</v>
-      </c>
-      <c r="B6" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B7" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B8" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>
@@ -1464,15 +1509,15 @@
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>161</v>
+      </c>
+      <c r="B3" t="s">
         <v>164</v>
-      </c>
-      <c r="B3" t="s">
-        <v>167</v>
       </c>
     </row>
   </sheetData>
@@ -1515,31 +1560,31 @@
         <v>25</v>
       </c>
       <c r="B3" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>165</v>
+      </c>
+      <c r="B4" t="s">
         <v>168</v>
-      </c>
-      <c r="B4" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>166</v>
+      </c>
+      <c r="B5" t="s">
         <v>169</v>
-      </c>
-      <c r="B5" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>167</v>
+      </c>
+      <c r="B6" t="s">
         <v>170</v>
-      </c>
-      <c r="B6" t="s">
-        <v>173</v>
       </c>
     </row>
   </sheetData>
@@ -1579,7 +1624,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B3" t="s">
         <v>79</v>
@@ -1590,7 +1635,7 @@
         <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1598,7 +1643,7 @@
         <v>70</v>
       </c>
       <c r="B5" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
   </sheetData>
@@ -1633,7 +1678,7 @@
         <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1646,7 +1691,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B4" t="s">
         <v>79</v>
@@ -1657,15 +1702,15 @@
         <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B6" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -1673,7 +1718,7 @@
         <v>71</v>
       </c>
       <c r="B7" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
   </sheetData>
@@ -1708,7 +1753,7 @@
         <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1716,12 +1761,12 @@
         <v>66</v>
       </c>
       <c r="B3" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B4" t="s">
         <v>79</v>
@@ -1732,7 +1777,7 @@
         <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1840,7 +1885,7 @@
         <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1848,12 +1893,12 @@
         <v>66</v>
       </c>
       <c r="B3" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B4" t="s">
         <v>79</v>
@@ -1864,7 +1909,7 @@
         <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -2038,18 +2083,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C534D12-2EFF-44CC-BEBB-F36901043652}">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.42578125" customWidth="1"/>
+    <col min="1" max="1" width="29.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="62.42578125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="52.140625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="104.28515625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="52.140625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="119.85546875" style="3" customWidth="1"/>
     <col min="6" max="6" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2058,10 +2103,10 @@
         <v>8</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>112</v>
+        <v>122</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>111</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>9</v>
@@ -2069,16 +2114,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>193</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>196</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>198</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>197</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2086,13 +2131,13 @@
         <v>10</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="C3" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>101</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -2102,7 +2147,7 @@
       <c r="B4" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="5" t="s">
         <v>99</v>
       </c>
       <c r="D4" s="3" t="s">
@@ -2116,151 +2161,207 @@
       <c r="B5" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="5" t="s">
         <v>100</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="C6" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>109</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>255</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>105</v>
+        <v>260</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>261</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="105" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>256</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>106</v>
+        <v>262</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>263</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="210" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>257</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>107</v>
+        <v>262</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>263</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>134</v>
+        <v>272</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>258</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>108</v>
+        <v>266</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>267</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>139</v>
+        <v>265</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>110</v>
+        <v>14</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>105</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B12" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="C12" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B13" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>132</v>
-      </c>
-      <c r="C13" s="6">
-        <v>0.5</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="C16" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>197</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>200</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>208</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="B18" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>204</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>205</v>
+      <c r="C18" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>259</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>270</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>271</v>
       </c>
     </row>
   </sheetData>
@@ -2293,66 +2394,66 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B2" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B3" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B4" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B5" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B6" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B7" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B8" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B9" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -2360,7 +2461,7 @@
         <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -2368,7 +2469,7 @@
         <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -2376,7 +2477,7 @@
         <v>15</v>
       </c>
       <c r="B12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -2384,7 +2485,7 @@
         <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -2392,7 +2493,7 @@
         <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -2400,7 +2501,7 @@
         <v>16</v>
       </c>
       <c r="B15" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -2408,7 +2509,7 @@
         <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -2416,7 +2517,7 @@
         <v>18</v>
       </c>
       <c r="B17" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -2424,7 +2525,7 @@
         <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -2432,7 +2533,7 @@
         <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -2440,23 +2541,23 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B21" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B22" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
   </sheetData>
@@ -2468,7 +2569,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16A05A0A-C7D1-40EE-9E15-74F73361602C}">
   <dimension ref="A1:C39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
@@ -2484,427 +2585,427 @@
         <v>10</v>
       </c>
       <c r="B1" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="C1" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>220</v>
-      </c>
-      <c r="B2" s="7">
+        <v>217</v>
+      </c>
+      <c r="B2" s="6">
         <v>44422</v>
       </c>
-      <c r="C2" s="7">
+      <c r="C2" s="6">
         <v>44561</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>221</v>
-      </c>
-      <c r="B3" s="7">
+        <v>218</v>
+      </c>
+      <c r="B3" s="6">
         <v>44751</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="6">
         <v>44804</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>222</v>
-      </c>
-      <c r="B4" s="7">
+        <v>219</v>
+      </c>
+      <c r="B4" s="6">
         <v>44562</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="6">
         <v>44620</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>223</v>
-      </c>
-      <c r="B5" s="7">
+        <v>220</v>
+      </c>
+      <c r="B5" s="6">
         <v>44709</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="6">
         <v>44752</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>224</v>
-      </c>
-      <c r="B6" s="7">
+        <v>221</v>
+      </c>
+      <c r="B6" s="6">
         <v>44348</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="6">
         <v>44392</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>225</v>
-      </c>
-      <c r="B7" s="7">
+        <v>222</v>
+      </c>
+      <c r="B7" s="6">
         <v>44713</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="6">
         <v>44757</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>226</v>
-      </c>
-      <c r="B8" s="7">
+        <v>223</v>
+      </c>
+      <c r="B8" s="6">
         <v>44682</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C8" s="6">
         <v>44712</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>227</v>
-      </c>
-      <c r="B9" s="7">
+        <v>224</v>
+      </c>
+      <c r="B9" s="6">
         <v>44345</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C9" s="6">
         <v>44395</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>228</v>
-      </c>
-      <c r="B10" s="7">
+        <v>225</v>
+      </c>
+      <c r="B10" s="6">
         <v>44562</v>
       </c>
-      <c r="C10" s="7">
+      <c r="C10" s="6">
         <v>44620</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>229</v>
-      </c>
-      <c r="B11" s="7">
+        <v>226</v>
+      </c>
+      <c r="B11" s="6">
         <v>44743</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C11" s="6">
         <v>44880</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>230</v>
-      </c>
-      <c r="B12" s="7">
+        <v>227</v>
+      </c>
+      <c r="B12" s="6">
         <v>44789</v>
       </c>
-      <c r="C12" s="7">
+      <c r="C12" s="6">
         <v>44834</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>231</v>
-      </c>
-      <c r="B13" s="7">
+        <v>228</v>
+      </c>
+      <c r="B13" s="6">
         <v>44757</v>
       </c>
-      <c r="C13" s="7">
+      <c r="C13" s="6">
         <v>44804</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>232</v>
-      </c>
-      <c r="B14" s="7">
+        <v>229</v>
+      </c>
+      <c r="B14" s="6">
         <v>44805</v>
       </c>
-      <c r="C14" s="7">
+      <c r="C14" s="6">
         <v>44910</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>233</v>
-      </c>
-      <c r="B15" s="7">
+        <v>230</v>
+      </c>
+      <c r="B15" s="6">
         <v>44728</v>
       </c>
-      <c r="C15" s="7">
+      <c r="C15" s="6">
         <v>44771</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>234</v>
-      </c>
-      <c r="B16" s="7">
+        <v>231</v>
+      </c>
+      <c r="B16" s="6">
         <v>44531</v>
       </c>
-      <c r="C16" s="7">
+      <c r="C16" s="6">
         <v>44607</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>235</v>
-      </c>
-      <c r="B17" s="7">
+        <v>232</v>
+      </c>
+      <c r="B17" s="6">
         <v>44805</v>
       </c>
-      <c r="C17" s="7">
+      <c r="C17" s="6">
         <v>44957</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>236</v>
-      </c>
-      <c r="B18" s="7">
+        <v>233</v>
+      </c>
+      <c r="B18" s="6">
         <v>44228</v>
       </c>
-      <c r="C18" s="7">
+      <c r="C18" s="6">
         <v>44301</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>237</v>
-      </c>
-      <c r="B19" s="7">
+        <v>234</v>
+      </c>
+      <c r="B19" s="6">
         <v>44709</v>
       </c>
-      <c r="C19" s="7">
+      <c r="C19" s="6">
         <v>44804</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>238</v>
-      </c>
-      <c r="B20" s="7">
+        <v>235</v>
+      </c>
+      <c r="B20" s="6">
         <v>44835</v>
       </c>
-      <c r="C20" s="7">
+      <c r="C20" s="6">
         <v>44972</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>239</v>
-      </c>
-      <c r="B21" s="7">
+        <v>236</v>
+      </c>
+      <c r="B21" s="6">
         <v>44820</v>
       </c>
-      <c r="C21" s="7">
+      <c r="C21" s="6">
         <v>44895</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>240</v>
-      </c>
-      <c r="B22" s="7">
+        <v>237</v>
+      </c>
+      <c r="B22" s="6">
         <v>44805</v>
       </c>
-      <c r="C22" s="7">
+      <c r="C22" s="6">
         <v>44895</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>241</v>
-      </c>
-      <c r="B23" s="7">
+        <v>238</v>
+      </c>
+      <c r="B23" s="6">
         <v>44455</v>
       </c>
-      <c r="C23" s="7">
+      <c r="C23" s="6">
         <v>44530</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>242</v>
-      </c>
-      <c r="B24" s="7">
+        <v>239</v>
+      </c>
+      <c r="B24" s="6">
         <v>44348</v>
       </c>
-      <c r="C24" s="7">
+      <c r="C24" s="6">
         <v>44392</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>243</v>
-      </c>
-      <c r="B25" s="7">
+        <v>240</v>
+      </c>
+      <c r="B25" s="6">
         <v>44713</v>
       </c>
-      <c r="C25" s="7">
+      <c r="C25" s="6">
         <v>44757</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>244</v>
-      </c>
-      <c r="B26" s="7">
+        <v>241</v>
+      </c>
+      <c r="B26" s="6">
         <v>44896</v>
       </c>
-      <c r="C26" s="7">
+      <c r="C26" s="6">
         <v>44972</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>245</v>
-      </c>
-      <c r="B27" s="7">
+        <v>242</v>
+      </c>
+      <c r="B27" s="6">
         <v>44896</v>
       </c>
-      <c r="C27" s="7">
+      <c r="C27" s="6">
         <v>44972</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>246</v>
-      </c>
-      <c r="B28" s="7">
+        <v>243</v>
+      </c>
+      <c r="B28" s="6">
         <v>44896</v>
       </c>
-      <c r="C28" s="7">
+      <c r="C28" s="6">
         <v>44957</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>247</v>
-      </c>
-      <c r="B29" s="7">
+        <v>244</v>
+      </c>
+      <c r="B29" s="6">
         <v>44531</v>
       </c>
-      <c r="C29" s="7">
+      <c r="C29" s="6">
         <v>44592</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>248</v>
-      </c>
-      <c r="B30" s="7">
+        <v>245</v>
+      </c>
+      <c r="B30" s="6">
         <v>44583</v>
       </c>
-      <c r="C30" s="7">
+      <c r="C30" s="6">
         <v>44607</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>249</v>
-      </c>
-      <c r="B31" s="7">
+        <v>246</v>
+      </c>
+      <c r="B31" s="6">
         <v>44562</v>
       </c>
-      <c r="C31" s="7">
+      <c r="C31" s="6">
         <v>44592</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>250</v>
-      </c>
-      <c r="B32" s="7">
+        <v>247</v>
+      </c>
+      <c r="B32" s="6">
         <v>44911</v>
       </c>
-      <c r="C32" s="7">
+      <c r="C32" s="6">
         <v>45016</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>251</v>
-      </c>
-      <c r="B33" s="7">
+        <v>248</v>
+      </c>
+      <c r="B33" s="6">
         <v>44911</v>
       </c>
-      <c r="C33" s="7">
+      <c r="C33" s="6">
         <v>45016</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>252</v>
-      </c>
-      <c r="B34" s="7">
+        <v>249</v>
+      </c>
+      <c r="B34" s="6">
         <v>44835</v>
       </c>
-      <c r="C34" s="7">
+      <c r="C34" s="6">
         <v>44911</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>253</v>
-      </c>
-      <c r="B35" s="7">
+        <v>250</v>
+      </c>
+      <c r="B35" s="6">
         <v>44805</v>
       </c>
-      <c r="C35" s="7">
+      <c r="C35" s="6">
         <v>44911</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>254</v>
-      </c>
-      <c r="B36" s="7">
+        <v>251</v>
+      </c>
+      <c r="B36" s="6">
         <v>44820</v>
       </c>
-      <c r="C36" s="7">
+      <c r="C36" s="6">
         <v>44911</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>255</v>
-      </c>
-      <c r="B37" s="7">
+        <v>252</v>
+      </c>
+      <c r="B37" s="6">
         <v>44910</v>
       </c>
-      <c r="C37" s="7">
+      <c r="C37" s="6">
         <v>45016</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>256</v>
-      </c>
-      <c r="B38" s="7">
+        <v>253</v>
+      </c>
+      <c r="B38" s="6">
         <v>44927</v>
       </c>
-      <c r="C38" s="7">
+      <c r="C38" s="6">
         <v>44957</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>257</v>
-      </c>
-      <c r="B39" s="7">
+        <v>254</v>
+      </c>
+      <c r="B39" s="6">
         <v>44958</v>
       </c>
-      <c r="C39" s="7">
+      <c r="C39" s="6">
         <v>45031</v>
       </c>
     </row>
@@ -3101,50 +3202,50 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B3" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B4" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B5" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B6" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B8" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -3152,39 +3253,39 @@
         <v>66</v>
       </c>
       <c r="B9" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B10" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B11" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B12" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B13" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Commit to catch up on outstanding edits to functions - circle back to review these soon!
</commit_message>
<xml_diff>
--- a/documentation_files/documentation_tables.xlsx
+++ b/documentation_files/documentation_tables.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stateofwa-my.sharepoint.com/personal/evan_booher_dfw_wa_gov/Documents/code/CreelEstimates/documentation_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="594" documentId="13_ncr:1_{06BDCB52-A10A-4652-9501-BAA58E581D65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{302421DA-0B90-4B17-BB60-8A31AA26AC16}"/>
+  <xr:revisionPtr revIDLastSave="655" documentId="13_ncr:1_{06BDCB52-A10A-4652-9501-BAA58E581D65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{32C718EE-ED94-4DA4-A7B0-5CFD878768FF}"/>
   <bookViews>
-    <workbookView xWindow="2580" yWindow="1680" windowWidth="25560" windowHeight="13050" firstSheet="1" activeTab="4" xr2:uid="{D87A213F-20EA-453F-96F1-E2F9D588DE08}"/>
+    <workbookView xWindow="1894" yWindow="1586" windowWidth="29546" windowHeight="13380" xr2:uid="{D87A213F-20EA-453F-96F1-E2F9D588DE08}"/>
   </bookViews>
   <sheets>
-    <sheet name="design_stratification" sheetId="7" r:id="rId1"/>
+    <sheet name="estimate_strata" sheetId="18" r:id="rId1"/>
     <sheet name="pre_analysis_checklist" sheetId="1" r:id="rId2"/>
     <sheet name="YAML_parameters" sheetId="2" r:id="rId3"/>
     <sheet name="YAML_param_options" sheetId="9" r:id="rId4"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="249">
   <si>
     <t>Data is stored in the creel database and accessible from data.wa.gov</t>
   </si>
@@ -222,18 +222,12 @@
     <t>time-period</t>
   </si>
   <si>
-    <t>options</t>
-  </si>
-  <si>
     <t>weekday, weekend</t>
   </si>
   <si>
     <t>bank, boat</t>
   </si>
   <si>
-    <t>varies by estimation method; daily, week, month, "duration"</t>
-  </si>
-  <si>
     <t>Index value representing the number of distinct index effort counts within a day at a given location</t>
   </si>
   <si>
@@ -591,54 +585,12 @@
     <t>Degrees of freedom stratified by section_num and angler_final; only applicable to "duration" option of paramter period_pe</t>
   </si>
   <si>
-    <t>index count type</t>
-  </si>
-  <si>
-    <t>effort count event</t>
-  </si>
-  <si>
-    <t>Categorical assignment of the objects being counted during index effort counts</t>
-  </si>
-  <si>
-    <t>Vehicle Only, Trailers Only, Bank Angler, Boat Angler</t>
-  </si>
-  <si>
-    <t>Temporal grouping of index effort counts associated with a scheduled count</t>
-  </si>
-  <si>
     <t>day-type</t>
   </si>
   <si>
     <t>angler-type</t>
   </si>
   <si>
-    <t>The type of survey completed during a scheduled index effort count</t>
-  </si>
-  <si>
-    <t xml:space="preserve">census, index </t>
-  </si>
-  <si>
-    <t>angler trip</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sample unit encompassing the trip information collected from a complete interview with an angler group </t>
-  </si>
-  <si>
-    <t>Specification of the “day type” used to aggregate n days within a week</t>
-  </si>
-  <si>
-    <t>Specification of the time step used to aggregate n days of observations from creel surveys</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Specification of the spatial domain used to aggregate observations from individual survey locations. A section contains one or more sites where effort counts and interviews occur. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Categorical assignment of the angler effort and catch based on a combinaton of observed fishing location and reported method used to access the fishery area </t>
-  </si>
-  <si>
-    <t>angler groups are either defined as the total group size (default) or the total angler count</t>
-  </si>
-  <si>
     <t>project_name</t>
   </si>
   <si>
@@ -823,6 +775,27 @@
   </si>
   <si>
     <t>Skagit winter steelhead 2023</t>
+  </si>
+  <si>
+    <t>stratum categories</t>
+  </si>
+  <si>
+    <t>varies by estimation method; daily, week, month, "duration" (single aggregated temporal stratum)</t>
+  </si>
+  <si>
+    <t>Specification of the time period assigned to creel data aggregated at the primary temporal unit of a day</t>
+  </si>
+  <si>
+    <t>Specification of the "day type" assigned to creel data aggregated at the primary temporal unit of a day</t>
+  </si>
+  <si>
+    <t>Categorical assignment of creel effort and angler interview data corresponding to observed fishing location and observed means to access the fishery (effort counts) and reported methods used to access fishing locations (interviews)</t>
+  </si>
+  <si>
+    <t>Specification of the spatial domain used to aggregate observations from individual survey locations. A section contains one or more sites where effort counts and interviews occur.</t>
+  </si>
+  <si>
+    <t>stratum field</t>
   </si>
 </sst>
 </file>
@@ -830,7 +803,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -917,7 +890,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1234,117 +1207,73 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8884888-2887-40E7-9CF4-425C1A207D31}">
-  <dimension ref="A1:C9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C2C2C09-FB49-4B37-9B1D-A348ADC7C4D5}">
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M15" sqref="M15:M16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="2" width="160.42578125" customWidth="1"/>
-    <col min="3" max="3" width="91.5703125" customWidth="1"/>
+    <col min="2" max="2" width="109.84375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="91.53515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B1" t="s">
+        <v>248</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>56</v>
       </c>
-      <c r="B2" t="s">
-        <v>192</v>
+      <c r="B2" s="3" t="s">
+        <v>244</v>
       </c>
       <c r="C2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>185</v>
-      </c>
-      <c r="B3" t="s">
-        <v>191</v>
+        <v>178</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>245</v>
       </c>
       <c r="C3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A4" t="s">
+        <v>179</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="C4" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>186</v>
-      </c>
-      <c r="B4" t="s">
-        <v>194</v>
-      </c>
-      <c r="C4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>77</v>
-      </c>
-      <c r="B5" t="s">
-        <v>193</v>
+        <v>75</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>247</v>
       </c>
       <c r="C5" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>180</v>
-      </c>
-      <c r="B6" t="s">
-        <v>182</v>
-      </c>
-      <c r="C6" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>181</v>
-      </c>
-      <c r="B7" t="s">
-        <v>184</v>
-      </c>
-      <c r="C7" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>181</v>
-      </c>
-      <c r="B8" t="s">
-        <v>187</v>
-      </c>
-      <c r="C8" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>189</v>
-      </c>
-      <c r="B9" t="s">
-        <v>190</v>
-      </c>
-      <c r="C9" t="s">
-        <v>195</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -1361,13 +1290,13 @@
       <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="44.5703125" customWidth="1"/>
-    <col min="2" max="2" width="106.85546875" customWidth="1"/>
+    <col min="1" max="1" width="44.53515625" customWidth="1"/>
+    <col min="2" max="2" width="106.84375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>21</v>
       </c>
@@ -1375,23 +1304,23 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B3" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -1399,36 +1328,36 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
+        <v>157</v>
+      </c>
+      <c r="B6" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A7" t="s">
+        <v>158</v>
+      </c>
+      <c r="B7" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A8" t="s">
         <v>159</v>
       </c>
-      <c r="B6" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>160</v>
-      </c>
-      <c r="B7" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="B8" t="s">
         <v>161</v>
-      </c>
-      <c r="B8" t="s">
-        <v>163</v>
       </c>
     </row>
   </sheetData>
@@ -1444,14 +1373,14 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="22.28515625" customWidth="1"/>
-    <col min="2" max="2" width="159.7109375" customWidth="1"/>
-    <col min="3" max="3" width="125.5703125" customWidth="1"/>
+    <col min="1" max="1" width="22.3046875" customWidth="1"/>
+    <col min="2" max="2" width="159.69140625" customWidth="1"/>
+    <col min="3" max="3" width="125.53515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>21</v>
       </c>
@@ -1459,20 +1388,20 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>25</v>
       </c>
       <c r="B2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
+        <v>162</v>
+      </c>
+      <c r="B3" t="s">
         <v>165</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>164</v>
-      </c>
-      <c r="B3" t="s">
-        <v>167</v>
       </c>
     </row>
   </sheetData>
@@ -1488,13 +1417,13 @@
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" customWidth="1"/>
-    <col min="2" max="2" width="161.5703125" customWidth="1"/>
+    <col min="1" max="1" width="18.3046875" customWidth="1"/>
+    <col min="2" max="2" width="161.53515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>21</v>
       </c>
@@ -1502,44 +1431,44 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>25</v>
       </c>
       <c r="B3" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
+        <v>166</v>
+      </c>
+      <c r="B4" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A5" t="s">
+        <v>167</v>
+      </c>
+      <c r="B5" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A6" t="s">
         <v>168</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B6" t="s">
         <v>171</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>169</v>
-      </c>
-      <c r="B5" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>170</v>
-      </c>
-      <c r="B6" t="s">
-        <v>173</v>
       </c>
     </row>
   </sheetData>
@@ -1555,13 +1484,13 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" customWidth="1"/>
-    <col min="2" max="2" width="89.5703125" customWidth="1"/>
+    <col min="1" max="1" width="15.84375" customWidth="1"/>
+    <col min="2" max="2" width="89.53515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>21</v>
       </c>
@@ -1569,36 +1498,36 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>22</v>
       </c>
       <c r="B4" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" t="s">
         <v>174</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>70</v>
-      </c>
-      <c r="B5" t="s">
-        <v>176</v>
       </c>
     </row>
   </sheetData>
@@ -1614,13 +1543,13 @@
       <selection activeCell="B19" sqref="B18:B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" customWidth="1"/>
+    <col min="1" max="1" width="17.69140625" customWidth="1"/>
     <col min="2" max="2" width="114" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>21</v>
       </c>
@@ -1628,52 +1557,52 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B4" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
+        <v>175</v>
+      </c>
+      <c r="B6" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B7" t="s">
         <v>177</v>
-      </c>
-      <c r="B6" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>71</v>
-      </c>
-      <c r="B7" t="s">
-        <v>179</v>
       </c>
     </row>
   </sheetData>
@@ -1689,13 +1618,13 @@
       <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="23.42578125" customWidth="1"/>
-    <col min="2" max="2" width="147.42578125" customWidth="1"/>
+    <col min="1" max="1" width="23.3828125" customWidth="1"/>
+    <col min="2" max="2" width="147.3828125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>21</v>
       </c>
@@ -1703,108 +1632,108 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B3" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B4" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A8" t="s">
         <v>67</v>
       </c>
-      <c r="B6" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="B8" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A9" t="s">
         <v>68</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B9" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A10" t="s">
         <v>69</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B10" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A11" t="s">
         <v>70</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B11" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A12" t="s">
         <v>71</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B12" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A13" t="s">
         <v>72</v>
       </c>
-      <c r="B11" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="B13" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A14" t="s">
         <v>73</v>
       </c>
-      <c r="B12" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>74</v>
-      </c>
-      <c r="B13" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>75</v>
-      </c>
       <c r="B14" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -1821,13 +1750,13 @@
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
-    <col min="2" max="2" width="138.42578125" customWidth="1"/>
+    <col min="2" max="2" width="138.3828125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>21</v>
       </c>
@@ -1835,116 +1764,116 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B3" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B4" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>36</v>
       </c>
       <c r="B6" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B7" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
+        <v>86</v>
+      </c>
+      <c r="B8" t="s">
         <v>88</v>
       </c>
-      <c r="B8" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
+        <v>87</v>
+      </c>
+      <c r="B9" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A10" t="s">
+        <v>68</v>
+      </c>
+      <c r="B10" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A11" t="s">
+        <v>69</v>
+      </c>
+      <c r="B11" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A12" t="s">
+        <v>70</v>
+      </c>
+      <c r="B12" t="s">
         <v>89</v>
       </c>
-      <c r="B9" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>70</v>
-      </c>
-      <c r="B10" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A13" t="s">
         <v>71</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B13" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A14" t="s">
         <v>72</v>
       </c>
-      <c r="B12" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="B14" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A15" t="s">
         <v>73</v>
       </c>
-      <c r="B13" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>74</v>
-      </c>
-      <c r="B14" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>75</v>
-      </c>
       <c r="B15" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -1957,24 +1886,24 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="1" max="1" width="9.15234375" style="1"/>
     <col min="2" max="2" width="130" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="1"/>
-    <col min="4" max="4" width="19.28515625" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
+    <col min="3" max="3" width="9.15234375" style="1"/>
+    <col min="4" max="4" width="19.3046875" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.15234375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="B1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1982,7 +1911,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1990,7 +1919,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="15.9" x14ac:dyDescent="0.4">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1998,7 +1927,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" ht="15.9" x14ac:dyDescent="0.4">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -2006,7 +1935,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -2014,7 +1943,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" ht="15.9" x14ac:dyDescent="0.4">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -2022,7 +1951,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" ht="15.9" x14ac:dyDescent="0.4">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -2044,58 +1973,58 @@
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="24.42578125" customWidth="1"/>
-    <col min="2" max="2" width="62.42578125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="52.140625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="104.28515625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" customWidth="1"/>
+    <col min="1" max="1" width="24.3828125" customWidth="1"/>
+    <col min="2" max="2" width="62.3828125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="52.15234375" style="6" customWidth="1"/>
+    <col min="4" max="4" width="104.3046875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="11.3828125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>8</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>196</v>
+        <v>180</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>198</v>
+        <v>182</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>197</v>
+        <v>181</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -2103,13 +2032,13 @@
         <v>39</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -2117,150 +2046,150 @@
         <v>39</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>14</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>15</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>16</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>17</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>18</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>19</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>20</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C13" s="6">
         <v>0.5</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
-        <v>200</v>
+        <v>184</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>207</v>
+        <v>191</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>208</v>
+        <v>192</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
-        <v>203</v>
+        <v>187</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>206</v>
+        <v>190</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>204</v>
+        <v>188</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>205</v>
+        <v>189</v>
       </c>
     </row>
   </sheetData>
@@ -2274,189 +2203,189 @@
   <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="A9:B11"/>
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="25.7109375" customWidth="1"/>
+    <col min="1" max="1" width="25.69140625" customWidth="1"/>
     <col min="2" max="2" width="31" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>8</v>
       </c>
       <c r="B1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
+        <v>180</v>
+      </c>
+      <c r="B2" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
+        <v>180</v>
+      </c>
+      <c r="B3" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A4" t="s">
+        <v>180</v>
+      </c>
+      <c r="B4" t="s">
         <v>196</v>
       </c>
-      <c r="B2" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>196</v>
-      </c>
-      <c r="B3" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>196</v>
-      </c>
-      <c r="B4" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>196</v>
+        <v>180</v>
       </c>
       <c r="B5" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>196</v>
+        <v>180</v>
       </c>
       <c r="B6" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
-        <v>196</v>
+        <v>180</v>
       </c>
       <c r="B7" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
-        <v>196</v>
+        <v>180</v>
       </c>
       <c r="B8" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
-        <v>196</v>
+        <v>180</v>
       </c>
       <c r="B9" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>15</v>
       </c>
       <c r="B12" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>16</v>
       </c>
       <c r="B15" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>18</v>
       </c>
       <c r="B17" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
-        <v>200</v>
+        <v>184</v>
       </c>
       <c r="B21" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
-        <v>200</v>
+        <v>184</v>
       </c>
       <c r="B22" t="s">
-        <v>202</v>
+        <v>186</v>
       </c>
     </row>
   </sheetData>
@@ -2468,31 +2397,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16A05A0A-C7D1-40EE-9E15-74F73361602C}">
   <dimension ref="A1:C39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="45.7109375" customWidth="1"/>
-    <col min="2" max="2" width="19.28515625" customWidth="1"/>
+    <col min="1" max="1" width="45.69140625" customWidth="1"/>
+    <col min="2" max="2" width="19.3046875" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>10</v>
       </c>
       <c r="B1" t="s">
-        <v>218</v>
+        <v>202</v>
       </c>
       <c r="C1" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>220</v>
+        <v>204</v>
       </c>
       <c r="B2" s="7">
         <v>44422</v>
@@ -2501,9 +2430,9 @@
         <v>44561</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>221</v>
+        <v>205</v>
       </c>
       <c r="B3" s="7">
         <v>44751</v>
@@ -2512,9 +2441,9 @@
         <v>44804</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>222</v>
+        <v>206</v>
       </c>
       <c r="B4" s="7">
         <v>44562</v>
@@ -2523,9 +2452,9 @@
         <v>44620</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>223</v>
+        <v>207</v>
       </c>
       <c r="B5" s="7">
         <v>44709</v>
@@ -2534,9 +2463,9 @@
         <v>44752</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>224</v>
+        <v>208</v>
       </c>
       <c r="B6" s="7">
         <v>44348</v>
@@ -2545,9 +2474,9 @@
         <v>44392</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
-        <v>225</v>
+        <v>209</v>
       </c>
       <c r="B7" s="7">
         <v>44713</v>
@@ -2556,9 +2485,9 @@
         <v>44757</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
-        <v>226</v>
+        <v>210</v>
       </c>
       <c r="B8" s="7">
         <v>44682</v>
@@ -2567,9 +2496,9 @@
         <v>44712</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
-        <v>227</v>
+        <v>211</v>
       </c>
       <c r="B9" s="7">
         <v>44345</v>
@@ -2578,9 +2507,9 @@
         <v>44395</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
-        <v>228</v>
+        <v>212</v>
       </c>
       <c r="B10" s="7">
         <v>44562</v>
@@ -2589,9 +2518,9 @@
         <v>44620</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
-        <v>229</v>
+        <v>213</v>
       </c>
       <c r="B11" s="7">
         <v>44743</v>
@@ -2600,9 +2529,9 @@
         <v>44880</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
-        <v>230</v>
+        <v>214</v>
       </c>
       <c r="B12" s="7">
         <v>44789</v>
@@ -2611,9 +2540,9 @@
         <v>44834</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
-        <v>231</v>
+        <v>215</v>
       </c>
       <c r="B13" s="7">
         <v>44757</v>
@@ -2622,9 +2551,9 @@
         <v>44804</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
-        <v>232</v>
+        <v>216</v>
       </c>
       <c r="B14" s="7">
         <v>44805</v>
@@ -2633,9 +2562,9 @@
         <v>44910</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
-        <v>233</v>
+        <v>217</v>
       </c>
       <c r="B15" s="7">
         <v>44728</v>
@@ -2644,9 +2573,9 @@
         <v>44771</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
-        <v>234</v>
+        <v>218</v>
       </c>
       <c r="B16" s="7">
         <v>44531</v>
@@ -2655,9 +2584,9 @@
         <v>44607</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
-        <v>235</v>
+        <v>219</v>
       </c>
       <c r="B17" s="7">
         <v>44805</v>
@@ -2666,9 +2595,9 @@
         <v>44957</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
-        <v>236</v>
+        <v>220</v>
       </c>
       <c r="B18" s="7">
         <v>44228</v>
@@ -2677,9 +2606,9 @@
         <v>44301</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
-        <v>237</v>
+        <v>221</v>
       </c>
       <c r="B19" s="7">
         <v>44709</v>
@@ -2688,9 +2617,9 @@
         <v>44804</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
-        <v>238</v>
+        <v>222</v>
       </c>
       <c r="B20" s="7">
         <v>44835</v>
@@ -2699,9 +2628,9 @@
         <v>44972</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
-        <v>239</v>
+        <v>223</v>
       </c>
       <c r="B21" s="7">
         <v>44820</v>
@@ -2710,9 +2639,9 @@
         <v>44895</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
-        <v>240</v>
+        <v>224</v>
       </c>
       <c r="B22" s="7">
         <v>44805</v>
@@ -2721,9 +2650,9 @@
         <v>44895</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
-        <v>241</v>
+        <v>225</v>
       </c>
       <c r="B23" s="7">
         <v>44455</v>
@@ -2732,9 +2661,9 @@
         <v>44530</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
-        <v>242</v>
+        <v>226</v>
       </c>
       <c r="B24" s="7">
         <v>44348</v>
@@ -2743,9 +2672,9 @@
         <v>44392</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
-        <v>243</v>
+        <v>227</v>
       </c>
       <c r="B25" s="7">
         <v>44713</v>
@@ -2754,9 +2683,9 @@
         <v>44757</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
-        <v>244</v>
+        <v>228</v>
       </c>
       <c r="B26" s="7">
         <v>44896</v>
@@ -2765,9 +2694,9 @@
         <v>44972</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
-        <v>245</v>
+        <v>229</v>
       </c>
       <c r="B27" s="7">
         <v>44896</v>
@@ -2776,9 +2705,9 @@
         <v>44972</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
-        <v>246</v>
+        <v>230</v>
       </c>
       <c r="B28" s="7">
         <v>44896</v>
@@ -2787,9 +2716,9 @@
         <v>44957</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
-        <v>247</v>
+        <v>231</v>
       </c>
       <c r="B29" s="7">
         <v>44531</v>
@@ -2798,9 +2727,9 @@
         <v>44592</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
-        <v>248</v>
+        <v>232</v>
       </c>
       <c r="B30" s="7">
         <v>44583</v>
@@ -2809,9 +2738,9 @@
         <v>44607</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
-        <v>249</v>
+        <v>233</v>
       </c>
       <c r="B31" s="7">
         <v>44562</v>
@@ -2820,9 +2749,9 @@
         <v>44592</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
-        <v>250</v>
+        <v>234</v>
       </c>
       <c r="B32" s="7">
         <v>44911</v>
@@ -2831,9 +2760,9 @@
         <v>45016</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
-        <v>251</v>
+        <v>235</v>
       </c>
       <c r="B33" s="7">
         <v>44911</v>
@@ -2842,9 +2771,9 @@
         <v>45016</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
-        <v>252</v>
+        <v>236</v>
       </c>
       <c r="B34" s="7">
         <v>44835</v>
@@ -2853,9 +2782,9 @@
         <v>44911</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
-        <v>253</v>
+        <v>237</v>
       </c>
       <c r="B35" s="7">
         <v>44805</v>
@@ -2864,9 +2793,9 @@
         <v>44911</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A36" t="s">
-        <v>254</v>
+        <v>238</v>
       </c>
       <c r="B36" s="7">
         <v>44820</v>
@@ -2875,9 +2804,9 @@
         <v>44911</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A37" t="s">
-        <v>255</v>
+        <v>239</v>
       </c>
       <c r="B37" s="7">
         <v>44910</v>
@@ -2886,9 +2815,9 @@
         <v>45016</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A38" t="s">
-        <v>256</v>
+        <v>240</v>
       </c>
       <c r="B38" s="7">
         <v>44927</v>
@@ -2897,9 +2826,9 @@
         <v>44957</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A39" t="s">
-        <v>257</v>
+        <v>241</v>
       </c>
       <c r="B39" s="7">
         <v>44958</v>
@@ -2921,13 +2850,13 @@
       <selection activeCell="A5" sqref="A5:A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="26.5703125" customWidth="1"/>
-    <col min="2" max="2" width="119.140625" customWidth="1"/>
+    <col min="1" max="1" width="26.53515625" customWidth="1"/>
+    <col min="2" max="2" width="119.15234375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>21</v>
       </c>
@@ -2935,7 +2864,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -2943,15 +2872,15 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>22</v>
       </c>
       <c r="B3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -2959,7 +2888,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -2967,7 +2896,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -2975,7 +2904,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>27</v>
       </c>
@@ -2983,7 +2912,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>28</v>
       </c>
@@ -2991,7 +2920,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>29</v>
       </c>
@@ -2999,7 +2928,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>30</v>
       </c>
@@ -3007,7 +2936,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -3015,7 +2944,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>32</v>
       </c>
@@ -3023,7 +2952,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>33</v>
       </c>
@@ -3031,7 +2960,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>34</v>
       </c>
@@ -3039,23 +2968,23 @@
         <v>49</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>35</v>
       </c>
       <c r="B15" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>36</v>
       </c>
       <c r="B16" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>37</v>
       </c>
@@ -3077,13 +3006,13 @@
       <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
-    <col min="2" max="2" width="109.7109375" customWidth="1"/>
+    <col min="2" max="2" width="109.69140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>21</v>
       </c>
@@ -3091,7 +3020,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>24</v>
       </c>
@@ -3099,92 +3028,92 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
+        <v>138</v>
+      </c>
+      <c r="B3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A4" t="s">
+        <v>139</v>
+      </c>
+      <c r="B4" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A5" t="s">
         <v>140</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B5" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A6" t="s">
         <v>141</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B6" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A8" t="s">
+        <v>114</v>
+      </c>
+      <c r="B8" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A9" t="s">
+        <v>64</v>
+      </c>
+      <c r="B9" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A10" t="s">
         <v>142</v>
       </c>
-      <c r="B5" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="B10" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A11" t="s">
         <v>143</v>
       </c>
-      <c r="B6" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>115</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>116</v>
-      </c>
-      <c r="B8" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>66</v>
-      </c>
-      <c r="B9" t="s">
+      <c r="B11" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A12" t="s">
         <v>144</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B12" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A13" t="s">
         <v>145</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B13" t="s">
         <v>156</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>146</v>
-      </c>
-      <c r="B12" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>147</v>
-      </c>
-      <c r="B13" t="s">
-        <v>158</v>
       </c>
     </row>
   </sheetData>
@@ -3201,13 +3130,13 @@
       <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="23.140625" customWidth="1"/>
-    <col min="2" max="2" width="97.42578125" customWidth="1"/>
+    <col min="1" max="1" width="23.15234375" customWidth="1"/>
+    <col min="2" max="2" width="97.3828125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>21</v>
       </c>
@@ -3215,15 +3144,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -3231,28 +3160,28 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>51</v>
       </c>
       <c r="B4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>52</v>
       </c>
       <c r="B5" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>53</v>
       </c>
       <c r="B6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -3269,13 +3198,13 @@
       <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="131.28515625" customWidth="1"/>
+    <col min="1" max="1" width="15.69140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="131.3046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>21</v>
       </c>
@@ -3283,15 +3212,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -3299,23 +3228,23 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>54</v>
       </c>
       <c r="B4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>51</v>
       </c>
       <c r="B5" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -3323,7 +3252,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -3331,12 +3260,12 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>55</v>
       </c>
       <c r="B8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
revert faulty merge 0e83b904ca0f75189217d6741c189e2e8c9c7b04
</commit_message>
<xml_diff>
--- a/documentation_files/documentation_tables.xlsx
+++ b/documentation_files/documentation_tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stateofwa-my.sharepoint.com/personal/kale_bentley_dfw_wa_gov/Documents/Projects/Creel/GitHub/CreelEstimates/documentation_files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stateofwa-my.sharepoint.com/personal/evan_booher_dfw_wa_gov/Documents/code/CreelEstimates/documentation_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="642" documentId="13_ncr:1_{06BDCB52-A10A-4652-9501-BAA58E581D65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D2F6D855-881A-4181-A9EC-550790DD7EBF}"/>
+  <xr:revisionPtr revIDLastSave="594" documentId="13_ncr:1_{06BDCB52-A10A-4652-9501-BAA58E581D65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{302421DA-0B90-4B17-BB60-8A31AA26AC16}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="2" xr2:uid="{D87A213F-20EA-453F-96F1-E2F9D588DE08}"/>
+    <workbookView xWindow="2580" yWindow="1680" windowWidth="25560" windowHeight="13050" firstSheet="1" activeTab="4" xr2:uid="{D87A213F-20EA-453F-96F1-E2F9D588DE08}"/>
   </bookViews>
   <sheets>
     <sheet name="design_stratification" sheetId="7" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="258">
   <si>
     <t>Data is stored in the creel database and accessible from data.wa.gov</t>
   </si>
@@ -381,6 +381,12 @@
     <t>c(species = 'steelhead', life_stage = 'Adult', fin_mark = 'UM|AD', fate = 'Released')</t>
   </si>
   <si>
+    <t>"Vehicles/Trailers Only"</t>
+  </si>
+  <si>
+    <t>"Direct"</t>
+  </si>
+  <si>
     <t>example_input</t>
   </si>
   <si>
@@ -435,6 +441,12 @@
     <t>concatenation of character strings with convention 'name of day"</t>
   </si>
   <si>
+    <t>"Vehicles/Trailers Only", "Bank Angler/Boat Angler"</t>
+  </si>
+  <si>
+    <t>"Direct", "Indirect"</t>
+  </si>
+  <si>
     <t>numeric value in hours</t>
   </si>
   <si>
@@ -444,6 +456,12 @@
     <t>Time period for aggregation of observations for use in BSS analysis</t>
   </si>
   <si>
+    <t>The objects or anglers that are counted during index effort counts, either "Vehicle/Trailers Only" or "Bank Angler / Boat Angler"</t>
+  </si>
+  <si>
+    <t>Control option to use either observed census data ("Direct") or assumed values ("Indirect") to calculate the effort bias term ratio</t>
+  </si>
+  <si>
     <t xml:space="preserve">Character string with waterbody area, focal species, year / year-group used to fetch a subset of data for analysis </t>
   </si>
   <si>
@@ -805,62 +823,6 @@
   </si>
   <si>
     <t>Skagit winter steelhead 2023</t>
-  </si>
-  <si>
-    <t>study_design</t>
-  </si>
-  <si>
-    <t>boat_type_collapse</t>
-  </si>
-  <si>
-    <t>fish_location_determines_type</t>
-  </si>
-  <si>
-    <t>angler_type_kayak_pontoon</t>
-  </si>
-  <si>
-    <t>bss_model_file_name</t>
-  </si>
-  <si>
-    <t>"Standard", "Drano"</t>
-  </si>
-  <si>
-    <t>"Standard"</t>
-  </si>
-  <si>
-    <t>"Yes", "No"</t>
-  </si>
-  <si>
-    <t>"No"</t>
-  </si>
-  <si>
-    <t>Parameter/argument used in several prep_dwg_ and prep_inputs_pe_ functions denoting which study design was followed during data collection, which impacts how the data are wrangled and analyzed.  Currently, the CreelAnalysis scripts have updated to accommodate two approved study designs ("Standard", "Drano") such that estimates of effort and catch can be generated using both the PE and BSS models.</t>
-  </si>
-  <si>
-    <t>Parameter/argument used in several prep_dwg_ functions that controls whether a boat designated as a kayak, pontoon, or kick during an effort count or angler group interview should be designated as a boat or bank angler.</t>
-  </si>
-  <si>
-    <t>"bank", "boat"</t>
-  </si>
-  <si>
-    <t>"bank"</t>
-  </si>
-  <si>
-    <t>Parameter/argument used in several prep_dwg_ functions that controls whether all (potential) boat types (e.g., motor_boat, drift_boat) are collapsed (i.e., boat_type_collapse: "Yes") into a single boat type or kept separate (boat_type_collapse: "No").  If multiple boat types were enumerated/specified during effort counts and interviews, estimates of effort and catch can (and will) be generated for each unique boat type using the PE estimator if "boat_type_collapse" is set to "No".  However, the current version of the BSS model (updated in April 2024) only has two possible angler types (bank, boat).  Thus, to generate estimates using the BSS model, "boat_type_collapse" must be set to "Yes".</t>
-  </si>
-  <si>
-    <t>character string matching name of the desired BSS model contained within the "stan_models" folder</t>
-  </si>
-  <si>
-    <t>"BSS_creel_model_02_2024-04-03.stan"</t>
-  </si>
-  <si>
-    <t>parameter/argument used in the "fit_bss_dev" function when running/fitting a BSS model; 
-NOTE: data wrangling functions are designed to work with the most up-to-date model.  Therefore, the utility of this argument (i.e., having the ability to specify different BSS/stan models) may not be functional or needed.</t>
-  </si>
-  <si>
-    <t>Parameter/argument used in several prep_dwg_ functions that controls whether the observed fishing location for a given angler group during an effort count determines their angler type.  For instance, if fish_location_determines_type is set to Yes, a boat angler group observed fishing on the bank (i.e., their boat is pulled up on the bank) during an effort count would be designated as a bank angler in the analysis.  Conversely, if fish_location_determines_type is set to No, the angler type is determined by the presence/absence of a boat (i.e., watercraft) during the effort count regardless of where it was positioned during the effort count (i.e., a boat angler group is designated as a boat angler even if anglers were fishing from shore).  Similarly, this parameter/argument determines whether the field "fish_from_boat" (which is a field that is collected during interviews exclusively from boat anglers specifying where they spent the majority of the day fishing from: bank or boat) is used to determine the angler type.  If fish_location_determines_type is set to Yes then a boat angler interview can be designated as a bank angler is they reported fishing from the bank the majority of the day.  Conversely, if fish_location_determines_type is set to No then an angler group that has a boat during the interview will be designated as a boat angler regardless of how they responded to the "fish_from_boat" question.  
-NOTE: the "fish_from_boat" question/field is not asked in every creel.  Therefore, this argument can be deleted from the corresponding function is not appliable (the function will designate the argument as NA by default).</t>
   </si>
 </sst>
 </file>
@@ -868,7 +830,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -895,7 +857,6 @@
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -940,7 +901,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -951,9 +912,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1300,7 +1264,7 @@
         <v>56</v>
       </c>
       <c r="B2" t="s">
-        <v>186</v>
+        <v>192</v>
       </c>
       <c r="C2" t="s">
         <v>60</v>
@@ -1308,10 +1272,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="B3" t="s">
-        <v>185</v>
+        <v>191</v>
       </c>
       <c r="C3" t="s">
         <v>58</v>
@@ -1319,10 +1283,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
       <c r="B4" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="C4" t="s">
         <v>59</v>
@@ -1333,7 +1297,7 @@
         <v>77</v>
       </c>
       <c r="B5" t="s">
-        <v>187</v>
+        <v>193</v>
       </c>
       <c r="C5" t="s">
         <v>78</v>
@@ -1341,21 +1305,21 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B6" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
       <c r="C6" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="B7" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="C7" t="s">
         <v>51</v>
@@ -1363,24 +1327,24 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="B8" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="C8" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="B9" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="C9" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
     </row>
   </sheetData>
@@ -1421,10 +1385,10 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="B3" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1440,31 +1404,31 @@
         <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="B6" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="B7" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="B8" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
     </row>
   </sheetData>
@@ -1500,15 +1464,15 @@
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="B3" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
     </row>
   </sheetData>
@@ -1551,31 +1515,31 @@
         <v>25</v>
       </c>
       <c r="B3" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="B4" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="B5" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="B6" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
     </row>
   </sheetData>
@@ -1615,7 +1579,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="B3" t="s">
         <v>79</v>
@@ -1626,7 +1590,7 @@
         <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1634,7 +1598,7 @@
         <v>70</v>
       </c>
       <c r="B5" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
     </row>
   </sheetData>
@@ -1669,7 +1633,7 @@
         <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1682,7 +1646,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="B4" t="s">
         <v>79</v>
@@ -1693,15 +1657,15 @@
         <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="B6" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -1709,7 +1673,7 @@
         <v>71</v>
       </c>
       <c r="B7" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
     </row>
   </sheetData>
@@ -1744,7 +1708,7 @@
         <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1752,12 +1716,12 @@
         <v>66</v>
       </c>
       <c r="B3" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="B4" t="s">
         <v>79</v>
@@ -1768,7 +1732,7 @@
         <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1876,7 +1840,7 @@
         <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1884,12 +1848,12 @@
         <v>66</v>
       </c>
       <c r="B3" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="B4" t="s">
         <v>79</v>
@@ -1900,7 +1864,7 @@
         <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -2074,18 +2038,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C534D12-2EFF-44CC-BEBB-F36901043652}">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C9" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.42578125" customWidth="1"/>
     <col min="2" max="2" width="62.42578125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="52.140625" style="5" customWidth="1"/>
-    <col min="4" max="4" width="119.85546875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="52.140625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="104.28515625" style="3" customWidth="1"/>
     <col min="6" max="6" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2094,10 +2058,10 @@
         <v>8</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>110</v>
+        <v>123</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>112</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>9</v>
@@ -2105,16 +2069,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>191</v>
+        <v>198</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>197</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>193</v>
+        <v>199</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2122,13 +2086,13 @@
         <v>10</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="C3" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>101</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -2138,7 +2102,7 @@
       <c r="B4" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="6" t="s">
         <v>99</v>
       </c>
       <c r="D4" s="3" t="s">
@@ -2152,193 +2116,151 @@
       <c r="B5" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="6" t="s">
         <v>100</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="C6" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>109</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>252</v>
+        <v>14</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>257</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>258</v>
+        <v>124</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>105</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>253</v>
+        <v>15</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>259</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>260</v>
+        <v>125</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>106</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="210" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>254</v>
+        <v>16</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>259</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>260</v>
+        <v>126</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>107</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>269</v>
+        <v>134</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>255</v>
+        <v>17</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>263</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>264</v>
+        <v>129</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>108</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>262</v>
+        <v>139</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>105</v>
+        <v>18</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>110</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>106</v>
+        <v>131</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>111</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>107</v>
+        <v>132</v>
+      </c>
+      <c r="C13" s="6">
+        <v>0.5</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>200</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>108</v>
+        <v>207</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>208</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>133</v>
+        <v>209</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>20</v>
+        <v>203</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="C15" s="5">
-        <v>0.5</v>
+        <v>206</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>204</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>194</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>201</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>202</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>197</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>256</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>266</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>267</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>268</v>
+        <v>205</v>
       </c>
     </row>
   </sheetData>
@@ -2371,66 +2293,66 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="B2" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="B3" t="s">
-        <v>205</v>
+        <v>211</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="B4" t="s">
-        <v>206</v>
+        <v>212</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="B5" t="s">
-        <v>207</v>
+        <v>213</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="B6" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="B7" t="s">
-        <v>209</v>
+        <v>215</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="B8" t="s">
-        <v>210</v>
+        <v>216</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="B9" t="s">
-        <v>211</v>
+        <v>217</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -2438,7 +2360,7 @@
         <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -2446,7 +2368,7 @@
         <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -2454,7 +2376,7 @@
         <v>15</v>
       </c>
       <c r="B12" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -2462,7 +2384,7 @@
         <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -2470,7 +2392,7 @@
         <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -2478,7 +2400,7 @@
         <v>16</v>
       </c>
       <c r="B15" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -2486,7 +2408,7 @@
         <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -2494,7 +2416,7 @@
         <v>18</v>
       </c>
       <c r="B17" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -2502,7 +2424,7 @@
         <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -2510,7 +2432,7 @@
         <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -2518,23 +2440,23 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="B21" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="B22" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
     </row>
   </sheetData>
@@ -2546,7 +2468,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16A05A0A-C7D1-40EE-9E15-74F73361602C}">
   <dimension ref="A1:C39"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
       <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
@@ -2562,427 +2484,427 @@
         <v>10</v>
       </c>
       <c r="B1" t="s">
-        <v>212</v>
+        <v>218</v>
       </c>
       <c r="C1" t="s">
-        <v>213</v>
+        <v>219</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>214</v>
-      </c>
-      <c r="B2" s="6">
+        <v>220</v>
+      </c>
+      <c r="B2" s="7">
         <v>44422</v>
       </c>
-      <c r="C2" s="6">
+      <c r="C2" s="7">
         <v>44561</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>215</v>
-      </c>
-      <c r="B3" s="6">
+        <v>221</v>
+      </c>
+      <c r="B3" s="7">
         <v>44751</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="7">
         <v>44804</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>216</v>
-      </c>
-      <c r="B4" s="6">
+        <v>222</v>
+      </c>
+      <c r="B4" s="7">
         <v>44562</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="7">
         <v>44620</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>217</v>
-      </c>
-      <c r="B5" s="6">
+        <v>223</v>
+      </c>
+      <c r="B5" s="7">
         <v>44709</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="7">
         <v>44752</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>218</v>
-      </c>
-      <c r="B6" s="6">
+        <v>224</v>
+      </c>
+      <c r="B6" s="7">
         <v>44348</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="7">
         <v>44392</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>219</v>
-      </c>
-      <c r="B7" s="6">
+        <v>225</v>
+      </c>
+      <c r="B7" s="7">
         <v>44713</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="7">
         <v>44757</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>220</v>
-      </c>
-      <c r="B8" s="6">
+        <v>226</v>
+      </c>
+      <c r="B8" s="7">
         <v>44682</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="7">
         <v>44712</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>221</v>
-      </c>
-      <c r="B9" s="6">
+        <v>227</v>
+      </c>
+      <c r="B9" s="7">
         <v>44345</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="7">
         <v>44395</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>222</v>
-      </c>
-      <c r="B10" s="6">
+        <v>228</v>
+      </c>
+      <c r="B10" s="7">
         <v>44562</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="7">
         <v>44620</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>223</v>
-      </c>
-      <c r="B11" s="6">
+        <v>229</v>
+      </c>
+      <c r="B11" s="7">
         <v>44743</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="7">
         <v>44880</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>224</v>
-      </c>
-      <c r="B12" s="6">
+        <v>230</v>
+      </c>
+      <c r="B12" s="7">
         <v>44789</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="7">
         <v>44834</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>225</v>
-      </c>
-      <c r="B13" s="6">
+        <v>231</v>
+      </c>
+      <c r="B13" s="7">
         <v>44757</v>
       </c>
-      <c r="C13" s="6">
+      <c r="C13" s="7">
         <v>44804</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>226</v>
-      </c>
-      <c r="B14" s="6">
+        <v>232</v>
+      </c>
+      <c r="B14" s="7">
         <v>44805</v>
       </c>
-      <c r="C14" s="6">
+      <c r="C14" s="7">
         <v>44910</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>227</v>
-      </c>
-      <c r="B15" s="6">
+        <v>233</v>
+      </c>
+      <c r="B15" s="7">
         <v>44728</v>
       </c>
-      <c r="C15" s="6">
+      <c r="C15" s="7">
         <v>44771</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>228</v>
-      </c>
-      <c r="B16" s="6">
+        <v>234</v>
+      </c>
+      <c r="B16" s="7">
         <v>44531</v>
       </c>
-      <c r="C16" s="6">
+      <c r="C16" s="7">
         <v>44607</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>229</v>
-      </c>
-      <c r="B17" s="6">
+        <v>235</v>
+      </c>
+      <c r="B17" s="7">
         <v>44805</v>
       </c>
-      <c r="C17" s="6">
+      <c r="C17" s="7">
         <v>44957</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>230</v>
-      </c>
-      <c r="B18" s="6">
+        <v>236</v>
+      </c>
+      <c r="B18" s="7">
         <v>44228</v>
       </c>
-      <c r="C18" s="6">
+      <c r="C18" s="7">
         <v>44301</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>231</v>
-      </c>
-      <c r="B19" s="6">
+        <v>237</v>
+      </c>
+      <c r="B19" s="7">
         <v>44709</v>
       </c>
-      <c r="C19" s="6">
+      <c r="C19" s="7">
         <v>44804</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>232</v>
-      </c>
-      <c r="B20" s="6">
+        <v>238</v>
+      </c>
+      <c r="B20" s="7">
         <v>44835</v>
       </c>
-      <c r="C20" s="6">
+      <c r="C20" s="7">
         <v>44972</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>233</v>
-      </c>
-      <c r="B21" s="6">
+        <v>239</v>
+      </c>
+      <c r="B21" s="7">
         <v>44820</v>
       </c>
-      <c r="C21" s="6">
+      <c r="C21" s="7">
         <v>44895</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>234</v>
-      </c>
-      <c r="B22" s="6">
+        <v>240</v>
+      </c>
+      <c r="B22" s="7">
         <v>44805</v>
       </c>
-      <c r="C22" s="6">
+      <c r="C22" s="7">
         <v>44895</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>235</v>
-      </c>
-      <c r="B23" s="6">
+        <v>241</v>
+      </c>
+      <c r="B23" s="7">
         <v>44455</v>
       </c>
-      <c r="C23" s="6">
+      <c r="C23" s="7">
         <v>44530</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>236</v>
-      </c>
-      <c r="B24" s="6">
+        <v>242</v>
+      </c>
+      <c r="B24" s="7">
         <v>44348</v>
       </c>
-      <c r="C24" s="6">
+      <c r="C24" s="7">
         <v>44392</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>237</v>
-      </c>
-      <c r="B25" s="6">
+        <v>243</v>
+      </c>
+      <c r="B25" s="7">
         <v>44713</v>
       </c>
-      <c r="C25" s="6">
+      <c r="C25" s="7">
         <v>44757</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>238</v>
-      </c>
-      <c r="B26" s="6">
+        <v>244</v>
+      </c>
+      <c r="B26" s="7">
         <v>44896</v>
       </c>
-      <c r="C26" s="6">
+      <c r="C26" s="7">
         <v>44972</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>239</v>
-      </c>
-      <c r="B27" s="6">
+        <v>245</v>
+      </c>
+      <c r="B27" s="7">
         <v>44896</v>
       </c>
-      <c r="C27" s="6">
+      <c r="C27" s="7">
         <v>44972</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>240</v>
-      </c>
-      <c r="B28" s="6">
+        <v>246</v>
+      </c>
+      <c r="B28" s="7">
         <v>44896</v>
       </c>
-      <c r="C28" s="6">
+      <c r="C28" s="7">
         <v>44957</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>241</v>
-      </c>
-      <c r="B29" s="6">
+        <v>247</v>
+      </c>
+      <c r="B29" s="7">
         <v>44531</v>
       </c>
-      <c r="C29" s="6">
+      <c r="C29" s="7">
         <v>44592</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>242</v>
-      </c>
-      <c r="B30" s="6">
+        <v>248</v>
+      </c>
+      <c r="B30" s="7">
         <v>44583</v>
       </c>
-      <c r="C30" s="6">
+      <c r="C30" s="7">
         <v>44607</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>243</v>
-      </c>
-      <c r="B31" s="6">
+        <v>249</v>
+      </c>
+      <c r="B31" s="7">
         <v>44562</v>
       </c>
-      <c r="C31" s="6">
+      <c r="C31" s="7">
         <v>44592</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>244</v>
-      </c>
-      <c r="B32" s="6">
+        <v>250</v>
+      </c>
+      <c r="B32" s="7">
         <v>44911</v>
       </c>
-      <c r="C32" s="6">
+      <c r="C32" s="7">
         <v>45016</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>245</v>
-      </c>
-      <c r="B33" s="6">
+        <v>251</v>
+      </c>
+      <c r="B33" s="7">
         <v>44911</v>
       </c>
-      <c r="C33" s="6">
+      <c r="C33" s="7">
         <v>45016</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>246</v>
-      </c>
-      <c r="B34" s="6">
+        <v>252</v>
+      </c>
+      <c r="B34" s="7">
         <v>44835</v>
       </c>
-      <c r="C34" s="6">
+      <c r="C34" s="7">
         <v>44911</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>247</v>
-      </c>
-      <c r="B35" s="6">
+        <v>253</v>
+      </c>
+      <c r="B35" s="7">
         <v>44805</v>
       </c>
-      <c r="C35" s="6">
+      <c r="C35" s="7">
         <v>44911</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>248</v>
-      </c>
-      <c r="B36" s="6">
+        <v>254</v>
+      </c>
+      <c r="B36" s="7">
         <v>44820</v>
       </c>
-      <c r="C36" s="6">
+      <c r="C36" s="7">
         <v>44911</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>249</v>
-      </c>
-      <c r="B37" s="6">
+        <v>255</v>
+      </c>
+      <c r="B37" s="7">
         <v>44910</v>
       </c>
-      <c r="C37" s="6">
+      <c r="C37" s="7">
         <v>45016</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>250</v>
-      </c>
-      <c r="B38" s="6">
+        <v>256</v>
+      </c>
+      <c r="B38" s="7">
         <v>44927</v>
       </c>
-      <c r="C38" s="6">
+      <c r="C38" s="7">
         <v>44957</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>251</v>
-      </c>
-      <c r="B39" s="6">
+        <v>257</v>
+      </c>
+      <c r="B39" s="7">
         <v>44958</v>
       </c>
-      <c r="C39" s="6">
+      <c r="C39" s="7">
         <v>45031</v>
       </c>
     </row>
@@ -3179,50 +3101,50 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="B3" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="B4" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="B5" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="B6" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B8" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -3230,39 +3152,39 @@
         <v>66</v>
       </c>
       <c r="B9" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="B10" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="B11" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="B12" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="B13" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "Model estimate storage feature"
</commit_message>
<xml_diff>
--- a/documentation_files/documentation_tables.xlsx
+++ b/documentation_files/documentation_tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stateofwa-my.sharepoint.com/personal/evan_booher_dfw_wa_gov/Documents/code/CreelEstimates/documentation_files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stateofwa-my.sharepoint.com/personal/kale_bentley_dfw_wa_gov/Documents/Projects/Creel/GitHub/CreelEstimates/documentation_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="594" documentId="13_ncr:1_{06BDCB52-A10A-4652-9501-BAA58E581D65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{302421DA-0B90-4B17-BB60-8A31AA26AC16}"/>
+  <xr:revisionPtr revIDLastSave="642" documentId="13_ncr:1_{06BDCB52-A10A-4652-9501-BAA58E581D65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D2F6D855-881A-4181-A9EC-550790DD7EBF}"/>
   <bookViews>
-    <workbookView xWindow="2580" yWindow="1680" windowWidth="25560" windowHeight="13050" firstSheet="1" activeTab="4" xr2:uid="{D87A213F-20EA-453F-96F1-E2F9D588DE08}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="2" xr2:uid="{D87A213F-20EA-453F-96F1-E2F9D588DE08}"/>
   </bookViews>
   <sheets>
     <sheet name="design_stratification" sheetId="7" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="270">
   <si>
     <t>Data is stored in the creel database and accessible from data.wa.gov</t>
   </si>
@@ -381,12 +381,6 @@
     <t>c(species = 'steelhead', life_stage = 'Adult', fin_mark = 'UM|AD', fate = 'Released')</t>
   </si>
   <si>
-    <t>"Vehicles/Trailers Only"</t>
-  </si>
-  <si>
-    <t>"Direct"</t>
-  </si>
-  <si>
     <t>example_input</t>
   </si>
   <si>
@@ -441,12 +435,6 @@
     <t>concatenation of character strings with convention 'name of day"</t>
   </si>
   <si>
-    <t>"Vehicles/Trailers Only", "Bank Angler/Boat Angler"</t>
-  </si>
-  <si>
-    <t>"Direct", "Indirect"</t>
-  </si>
-  <si>
     <t>numeric value in hours</t>
   </si>
   <si>
@@ -456,12 +444,6 @@
     <t>Time period for aggregation of observations for use in BSS analysis</t>
   </si>
   <si>
-    <t>The objects or anglers that are counted during index effort counts, either "Vehicle/Trailers Only" or "Bank Angler / Boat Angler"</t>
-  </si>
-  <si>
-    <t>Control option to use either observed census data ("Direct") or assumed values ("Indirect") to calculate the effort bias term ratio</t>
-  </si>
-  <si>
     <t xml:space="preserve">Character string with waterbody area, focal species, year / year-group used to fetch a subset of data for analysis </t>
   </si>
   <si>
@@ -823,6 +805,62 @@
   </si>
   <si>
     <t>Skagit winter steelhead 2023</t>
+  </si>
+  <si>
+    <t>study_design</t>
+  </si>
+  <si>
+    <t>boat_type_collapse</t>
+  </si>
+  <si>
+    <t>fish_location_determines_type</t>
+  </si>
+  <si>
+    <t>angler_type_kayak_pontoon</t>
+  </si>
+  <si>
+    <t>bss_model_file_name</t>
+  </si>
+  <si>
+    <t>"Standard", "Drano"</t>
+  </si>
+  <si>
+    <t>"Standard"</t>
+  </si>
+  <si>
+    <t>"Yes", "No"</t>
+  </si>
+  <si>
+    <t>"No"</t>
+  </si>
+  <si>
+    <t>Parameter/argument used in several prep_dwg_ and prep_inputs_pe_ functions denoting which study design was followed during data collection, which impacts how the data are wrangled and analyzed.  Currently, the CreelAnalysis scripts have updated to accommodate two approved study designs ("Standard", "Drano") such that estimates of effort and catch can be generated using both the PE and BSS models.</t>
+  </si>
+  <si>
+    <t>Parameter/argument used in several prep_dwg_ functions that controls whether a boat designated as a kayak, pontoon, or kick during an effort count or angler group interview should be designated as a boat or bank angler.</t>
+  </si>
+  <si>
+    <t>"bank", "boat"</t>
+  </si>
+  <si>
+    <t>"bank"</t>
+  </si>
+  <si>
+    <t>Parameter/argument used in several prep_dwg_ functions that controls whether all (potential) boat types (e.g., motor_boat, drift_boat) are collapsed (i.e., boat_type_collapse: "Yes") into a single boat type or kept separate (boat_type_collapse: "No").  If multiple boat types were enumerated/specified during effort counts and interviews, estimates of effort and catch can (and will) be generated for each unique boat type using the PE estimator if "boat_type_collapse" is set to "No".  However, the current version of the BSS model (updated in April 2024) only has two possible angler types (bank, boat).  Thus, to generate estimates using the BSS model, "boat_type_collapse" must be set to "Yes".</t>
+  </si>
+  <si>
+    <t>character string matching name of the desired BSS model contained within the "stan_models" folder</t>
+  </si>
+  <si>
+    <t>"BSS_creel_model_02_2024-04-03.stan"</t>
+  </si>
+  <si>
+    <t>parameter/argument used in the "fit_bss_dev" function when running/fitting a BSS model; 
+NOTE: data wrangling functions are designed to work with the most up-to-date model.  Therefore, the utility of this argument (i.e., having the ability to specify different BSS/stan models) may not be functional or needed.</t>
+  </si>
+  <si>
+    <t>Parameter/argument used in several prep_dwg_ functions that controls whether the observed fishing location for a given angler group during an effort count determines their angler type.  For instance, if fish_location_determines_type is set to Yes, a boat angler group observed fishing on the bank (i.e., their boat is pulled up on the bank) during an effort count would be designated as a bank angler in the analysis.  Conversely, if fish_location_determines_type is set to No, the angler type is determined by the presence/absence of a boat (i.e., watercraft) during the effort count regardless of where it was positioned during the effort count (i.e., a boat angler group is designated as a boat angler even if anglers were fishing from shore).  Similarly, this parameter/argument determines whether the field "fish_from_boat" (which is a field that is collected during interviews exclusively from boat anglers specifying where they spent the majority of the day fishing from: bank or boat) is used to determine the angler type.  If fish_location_determines_type is set to Yes then a boat angler interview can be designated as a bank angler is they reported fishing from the bank the majority of the day.  Conversely, if fish_location_determines_type is set to No then an angler group that has a boat during the interview will be designated as a boat angler regardless of how they responded to the "fish_from_boat" question.  
+NOTE: the "fish_from_boat" question/field is not asked in every creel.  Therefore, this argument can be deleted from the corresponding function is not appliable (the function will designate the argument as NA by default).</t>
   </si>
 </sst>
 </file>
@@ -830,7 +868,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -857,6 +895,7 @@
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -901,7 +940,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -912,12 +951,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1264,7 +1300,7 @@
         <v>56</v>
       </c>
       <c r="B2" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="C2" t="s">
         <v>60</v>
@@ -1272,10 +1308,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>179</v>
+      </c>
+      <c r="B3" t="s">
         <v>185</v>
-      </c>
-      <c r="B3" t="s">
-        <v>191</v>
       </c>
       <c r="C3" t="s">
         <v>58</v>
@@ -1283,10 +1319,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="B4" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="C4" t="s">
         <v>59</v>
@@ -1297,7 +1333,7 @@
         <v>77</v>
       </c>
       <c r="B5" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="C5" t="s">
         <v>78</v>
@@ -1305,21 +1341,21 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="B6" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="C6" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="B7" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="C7" t="s">
         <v>51</v>
@@ -1327,24 +1363,24 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>175</v>
+      </c>
+      <c r="B8" t="s">
         <v>181</v>
       </c>
-      <c r="B8" t="s">
-        <v>187</v>
-      </c>
       <c r="C8" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>183</v>
+      </c>
+      <c r="B9" t="s">
+        <v>184</v>
+      </c>
+      <c r="C9" t="s">
         <v>189</v>
-      </c>
-      <c r="B9" t="s">
-        <v>190</v>
-      </c>
-      <c r="C9" t="s">
-        <v>195</v>
       </c>
     </row>
   </sheetData>
@@ -1385,10 +1421,10 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="B3" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1404,31 +1440,31 @@
         <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="B6" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>154</v>
+      </c>
+      <c r="B7" t="s">
         <v>160</v>
-      </c>
-      <c r="B7" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="B8" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
     </row>
   </sheetData>
@@ -1464,15 +1500,15 @@
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="B3" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
     </row>
   </sheetData>
@@ -1515,31 +1551,31 @@
         <v>25</v>
       </c>
       <c r="B3" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="B4" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="B5" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="B6" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
   </sheetData>
@@ -1579,7 +1615,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="B3" t="s">
         <v>79</v>
@@ -1590,7 +1626,7 @@
         <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1598,7 +1634,7 @@
         <v>70</v>
       </c>
       <c r="B5" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
     </row>
   </sheetData>
@@ -1633,7 +1669,7 @@
         <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1646,7 +1682,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="B4" t="s">
         <v>79</v>
@@ -1657,15 +1693,15 @@
         <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="B6" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -1673,7 +1709,7 @@
         <v>71</v>
       </c>
       <c r="B7" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
     </row>
   </sheetData>
@@ -1708,7 +1744,7 @@
         <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1716,12 +1752,12 @@
         <v>66</v>
       </c>
       <c r="B3" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="B4" t="s">
         <v>79</v>
@@ -1732,7 +1768,7 @@
         <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1840,7 +1876,7 @@
         <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1848,12 +1884,12 @@
         <v>66</v>
       </c>
       <c r="B3" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="B4" t="s">
         <v>79</v>
@@ -1864,7 +1900,7 @@
         <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -2038,18 +2074,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C534D12-2EFF-44CC-BEBB-F36901043652}">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="C9" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.42578125" customWidth="1"/>
+    <col min="1" max="1" width="29.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="62.42578125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="52.140625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="104.28515625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="52.140625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="119.85546875" style="3" customWidth="1"/>
     <col min="6" max="6" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2058,10 +2094,10 @@
         <v>8</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>112</v>
+        <v>121</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>110</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>9</v>
@@ -2069,16 +2105,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>198</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>197</v>
+        <v>192</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>191</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2086,13 +2122,13 @@
         <v>10</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="C3" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>101</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -2102,7 +2138,7 @@
       <c r="B4" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="5" t="s">
         <v>99</v>
       </c>
       <c r="D4" s="3" t="s">
@@ -2116,151 +2152,193 @@
       <c r="B5" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="5" t="s">
         <v>100</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="C6" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>109</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>252</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>105</v>
+        <v>257</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>258</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>253</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>106</v>
+        <v>259</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>260</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="210" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>254</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>107</v>
+        <v>259</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>260</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>134</v>
+        <v>269</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>255</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>108</v>
+        <v>263</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>264</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>139</v>
+        <v>262</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="C11" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>19</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="C13" s="6">
-        <v>0.5</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>200</v>
+        <v>17</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>208</v>
+        <v>127</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>108</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>209</v>
+        <v>133</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="C15" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>194</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="D16" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>204</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>205</v>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>197</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>256</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>268</v>
       </c>
     </row>
   </sheetData>
@@ -2293,66 +2371,66 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="B2" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="B3" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="B4" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="B5" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="B6" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="B7" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="B8" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="B9" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -2360,7 +2438,7 @@
         <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -2368,7 +2446,7 @@
         <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -2376,7 +2454,7 @@
         <v>15</v>
       </c>
       <c r="B12" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -2384,7 +2462,7 @@
         <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -2392,7 +2470,7 @@
         <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -2400,7 +2478,7 @@
         <v>16</v>
       </c>
       <c r="B15" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -2408,7 +2486,7 @@
         <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -2416,7 +2494,7 @@
         <v>18</v>
       </c>
       <c r="B17" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -2424,7 +2502,7 @@
         <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -2432,7 +2510,7 @@
         <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -2440,23 +2518,23 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="B21" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="B22" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
     </row>
   </sheetData>
@@ -2468,7 +2546,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16A05A0A-C7D1-40EE-9E15-74F73361602C}">
   <dimension ref="A1:C39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
@@ -2484,427 +2562,427 @@
         <v>10</v>
       </c>
       <c r="B1" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="C1" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>220</v>
-      </c>
-      <c r="B2" s="7">
+        <v>214</v>
+      </c>
+      <c r="B2" s="6">
         <v>44422</v>
       </c>
-      <c r="C2" s="7">
+      <c r="C2" s="6">
         <v>44561</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>221</v>
-      </c>
-      <c r="B3" s="7">
+        <v>215</v>
+      </c>
+      <c r="B3" s="6">
         <v>44751</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="6">
         <v>44804</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>222</v>
-      </c>
-      <c r="B4" s="7">
+        <v>216</v>
+      </c>
+      <c r="B4" s="6">
         <v>44562</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="6">
         <v>44620</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>223</v>
-      </c>
-      <c r="B5" s="7">
+        <v>217</v>
+      </c>
+      <c r="B5" s="6">
         <v>44709</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="6">
         <v>44752</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>224</v>
-      </c>
-      <c r="B6" s="7">
+        <v>218</v>
+      </c>
+      <c r="B6" s="6">
         <v>44348</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="6">
         <v>44392</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>225</v>
-      </c>
-      <c r="B7" s="7">
+        <v>219</v>
+      </c>
+      <c r="B7" s="6">
         <v>44713</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="6">
         <v>44757</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>226</v>
-      </c>
-      <c r="B8" s="7">
+        <v>220</v>
+      </c>
+      <c r="B8" s="6">
         <v>44682</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C8" s="6">
         <v>44712</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>227</v>
-      </c>
-      <c r="B9" s="7">
+        <v>221</v>
+      </c>
+      <c r="B9" s="6">
         <v>44345</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C9" s="6">
         <v>44395</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>228</v>
-      </c>
-      <c r="B10" s="7">
+        <v>222</v>
+      </c>
+      <c r="B10" s="6">
         <v>44562</v>
       </c>
-      <c r="C10" s="7">
+      <c r="C10" s="6">
         <v>44620</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>229</v>
-      </c>
-      <c r="B11" s="7">
+        <v>223</v>
+      </c>
+      <c r="B11" s="6">
         <v>44743</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C11" s="6">
         <v>44880</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>230</v>
-      </c>
-      <c r="B12" s="7">
+        <v>224</v>
+      </c>
+      <c r="B12" s="6">
         <v>44789</v>
       </c>
-      <c r="C12" s="7">
+      <c r="C12" s="6">
         <v>44834</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>231</v>
-      </c>
-      <c r="B13" s="7">
+        <v>225</v>
+      </c>
+      <c r="B13" s="6">
         <v>44757</v>
       </c>
-      <c r="C13" s="7">
+      <c r="C13" s="6">
         <v>44804</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>232</v>
-      </c>
-      <c r="B14" s="7">
+        <v>226</v>
+      </c>
+      <c r="B14" s="6">
         <v>44805</v>
       </c>
-      <c r="C14" s="7">
+      <c r="C14" s="6">
         <v>44910</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>233</v>
-      </c>
-      <c r="B15" s="7">
+        <v>227</v>
+      </c>
+      <c r="B15" s="6">
         <v>44728</v>
       </c>
-      <c r="C15" s="7">
+      <c r="C15" s="6">
         <v>44771</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>234</v>
-      </c>
-      <c r="B16" s="7">
+        <v>228</v>
+      </c>
+      <c r="B16" s="6">
         <v>44531</v>
       </c>
-      <c r="C16" s="7">
+      <c r="C16" s="6">
         <v>44607</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>235</v>
-      </c>
-      <c r="B17" s="7">
+        <v>229</v>
+      </c>
+      <c r="B17" s="6">
         <v>44805</v>
       </c>
-      <c r="C17" s="7">
+      <c r="C17" s="6">
         <v>44957</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>236</v>
-      </c>
-      <c r="B18" s="7">
+        <v>230</v>
+      </c>
+      <c r="B18" s="6">
         <v>44228</v>
       </c>
-      <c r="C18" s="7">
+      <c r="C18" s="6">
         <v>44301</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>237</v>
-      </c>
-      <c r="B19" s="7">
+        <v>231</v>
+      </c>
+      <c r="B19" s="6">
         <v>44709</v>
       </c>
-      <c r="C19" s="7">
+      <c r="C19" s="6">
         <v>44804</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>238</v>
-      </c>
-      <c r="B20" s="7">
+        <v>232</v>
+      </c>
+      <c r="B20" s="6">
         <v>44835</v>
       </c>
-      <c r="C20" s="7">
+      <c r="C20" s="6">
         <v>44972</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>239</v>
-      </c>
-      <c r="B21" s="7">
+        <v>233</v>
+      </c>
+      <c r="B21" s="6">
         <v>44820</v>
       </c>
-      <c r="C21" s="7">
+      <c r="C21" s="6">
         <v>44895</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>240</v>
-      </c>
-      <c r="B22" s="7">
+        <v>234</v>
+      </c>
+      <c r="B22" s="6">
         <v>44805</v>
       </c>
-      <c r="C22" s="7">
+      <c r="C22" s="6">
         <v>44895</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>241</v>
-      </c>
-      <c r="B23" s="7">
+        <v>235</v>
+      </c>
+      <c r="B23" s="6">
         <v>44455</v>
       </c>
-      <c r="C23" s="7">
+      <c r="C23" s="6">
         <v>44530</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>242</v>
-      </c>
-      <c r="B24" s="7">
+        <v>236</v>
+      </c>
+      <c r="B24" s="6">
         <v>44348</v>
       </c>
-      <c r="C24" s="7">
+      <c r="C24" s="6">
         <v>44392</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>243</v>
-      </c>
-      <c r="B25" s="7">
+        <v>237</v>
+      </c>
+      <c r="B25" s="6">
         <v>44713</v>
       </c>
-      <c r="C25" s="7">
+      <c r="C25" s="6">
         <v>44757</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>244</v>
-      </c>
-      <c r="B26" s="7">
+        <v>238</v>
+      </c>
+      <c r="B26" s="6">
         <v>44896</v>
       </c>
-      <c r="C26" s="7">
+      <c r="C26" s="6">
         <v>44972</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>245</v>
-      </c>
-      <c r="B27" s="7">
+        <v>239</v>
+      </c>
+      <c r="B27" s="6">
         <v>44896</v>
       </c>
-      <c r="C27" s="7">
+      <c r="C27" s="6">
         <v>44972</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>246</v>
-      </c>
-      <c r="B28" s="7">
+        <v>240</v>
+      </c>
+      <c r="B28" s="6">
         <v>44896</v>
       </c>
-      <c r="C28" s="7">
+      <c r="C28" s="6">
         <v>44957</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>247</v>
-      </c>
-      <c r="B29" s="7">
+        <v>241</v>
+      </c>
+      <c r="B29" s="6">
         <v>44531</v>
       </c>
-      <c r="C29" s="7">
+      <c r="C29" s="6">
         <v>44592</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>248</v>
-      </c>
-      <c r="B30" s="7">
+        <v>242</v>
+      </c>
+      <c r="B30" s="6">
         <v>44583</v>
       </c>
-      <c r="C30" s="7">
+      <c r="C30" s="6">
         <v>44607</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>249</v>
-      </c>
-      <c r="B31" s="7">
+        <v>243</v>
+      </c>
+      <c r="B31" s="6">
         <v>44562</v>
       </c>
-      <c r="C31" s="7">
+      <c r="C31" s="6">
         <v>44592</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>250</v>
-      </c>
-      <c r="B32" s="7">
+        <v>244</v>
+      </c>
+      <c r="B32" s="6">
         <v>44911</v>
       </c>
-      <c r="C32" s="7">
+      <c r="C32" s="6">
         <v>45016</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>251</v>
-      </c>
-      <c r="B33" s="7">
+        <v>245</v>
+      </c>
+      <c r="B33" s="6">
         <v>44911</v>
       </c>
-      <c r="C33" s="7">
+      <c r="C33" s="6">
         <v>45016</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>252</v>
-      </c>
-      <c r="B34" s="7">
+        <v>246</v>
+      </c>
+      <c r="B34" s="6">
         <v>44835</v>
       </c>
-      <c r="C34" s="7">
+      <c r="C34" s="6">
         <v>44911</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>253</v>
-      </c>
-      <c r="B35" s="7">
+        <v>247</v>
+      </c>
+      <c r="B35" s="6">
         <v>44805</v>
       </c>
-      <c r="C35" s="7">
+      <c r="C35" s="6">
         <v>44911</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>254</v>
-      </c>
-      <c r="B36" s="7">
+        <v>248</v>
+      </c>
+      <c r="B36" s="6">
         <v>44820</v>
       </c>
-      <c r="C36" s="7">
+      <c r="C36" s="6">
         <v>44911</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>255</v>
-      </c>
-      <c r="B37" s="7">
+        <v>249</v>
+      </c>
+      <c r="B37" s="6">
         <v>44910</v>
       </c>
-      <c r="C37" s="7">
+      <c r="C37" s="6">
         <v>45016</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>256</v>
-      </c>
-      <c r="B38" s="7">
+        <v>250</v>
+      </c>
+      <c r="B38" s="6">
         <v>44927</v>
       </c>
-      <c r="C38" s="7">
+      <c r="C38" s="6">
         <v>44957</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>257</v>
-      </c>
-      <c r="B39" s="7">
+        <v>251</v>
+      </c>
+      <c r="B39" s="6">
         <v>44958</v>
       </c>
-      <c r="C39" s="7">
+      <c r="C39" s="6">
         <v>45031</v>
       </c>
     </row>
@@ -3101,50 +3179,50 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="B3" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="B4" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="B5" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="B6" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B8" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -3152,39 +3230,39 @@
         <v>66</v>
       </c>
       <c r="B9" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="B10" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="B11" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="B12" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="B13" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
     </row>
   </sheetData>

</xml_diff>